<commit_message>
update spreadsheets and rake task to use newer analysis gem
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="562" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -6747,8 +6747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -19346,7 +19346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating ami versions to latest in all excel projects.
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="562"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2445,10 +2445,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>1.11.0-rc3</t>
-  </si>
-  <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>1.12.4</t>
   </si>
 </sst>
 </file>
@@ -6748,7 +6748,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6806,7 +6806,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -6817,7 +6817,7 @@
         <v>468</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>470</v>

</xml_diff>

<commit_message>
adding argument to add runperiod in AddMonthlyJSONUtilityData/measure.rb
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$2:$AA$127</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2646" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="821">
   <si>
     <t>type</t>
   </si>
@@ -2497,6 +2497,12 @@
   </si>
   <si>
     <t>FALSE</t>
+  </si>
+  <si>
+    <t>Set RunPeriod</t>
+  </si>
+  <si>
+    <t>set_runperiod</t>
   </si>
 </sst>
 </file>
@@ -7226,11 +7232,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z199"/>
+  <dimension ref="A1:Z200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7559,60 +7565,60 @@
       </c>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="b">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B13" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>819</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>820</v>
+      </c>
+      <c r="F13" s="64"/>
+      <c r="G13" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>812</v>
+      </c>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B14" s="37" t="s">
         <v>813</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C14" s="37" t="s">
         <v>796</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D14" s="37" t="s">
         <v>796</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E14" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>797</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>798</v>
-      </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="31" t="s">
-        <v>732</v>
-      </c>
-      <c r="I14" s="31" t="s">
-        <v>814</v>
-      </c>
-      <c r="J14" s="31"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>164</v>
+        <v>798</v>
       </c>
       <c r="F15" s="64"/>
       <c r="G15" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -7621,17 +7627,17 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>803</v>
+        <v>164</v>
       </c>
       <c r="F16" s="64"/>
       <c r="G16" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="J16" s="31"/>
     </row>
@@ -7640,17 +7646,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>650</v>
+        <v>816</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7659,17 +7665,17 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>817</v>
+        <v>650</v>
       </c>
       <c r="J18" s="31"/>
     </row>
@@ -7678,17 +7684,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>733</v>
+        <v>807</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>734</v>
+        <v>808</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="31" t="s">
         <v>732</v>
       </c>
-      <c r="I19" s="48" t="s">
-        <v>765</v>
+      <c r="I19" s="31" t="s">
+        <v>817</v>
       </c>
       <c r="J19" s="31"/>
     </row>
@@ -7697,17 +7703,17 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F20" s="64"/>
       <c r="G20" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I20" s="48" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="J20" s="31"/>
     </row>
@@ -7716,199 +7722,200 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>810</v>
+        <v>735</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>811</v>
+        <v>736</v>
       </c>
       <c r="F21" s="64"/>
       <c r="G21" s="31" t="s">
+        <v>732</v>
+      </c>
+      <c r="I21" s="48" t="s">
+        <v>766</v>
+      </c>
+      <c r="J21" s="31"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>811</v>
+      </c>
+      <c r="F22" s="64"/>
+      <c r="G22" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I22" s="48" t="s">
         <v>818</v>
       </c>
-      <c r="J21" s="31"/>
-    </row>
-    <row r="22" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="b">
+      <c r="J22" s="31"/>
+    </row>
+    <row r="23" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B23" s="37" t="s">
         <v>646</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C23" s="37" t="s">
         <v>645</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D23" s="37" t="s">
         <v>645</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E23" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="1:18" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="b">
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="1:18" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B24" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C24" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="D24" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E24" s="45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="30" t="s">
+    <row r="25" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="64"/>
-      <c r="G24" s="30" t="s">
+      <c r="F25" s="64"/>
+      <c r="G25" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I24" s="30" t="s">
+      <c r="I25" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="30" t="s">
+      <c r="J25" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="P24" s="31"/>
-    </row>
-    <row r="25" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="40" t="s">
+      <c r="P25" s="31"/>
+    </row>
+    <row r="26" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D26" s="41" t="s">
         <v>681</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E26" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="40">
-        <v>0</v>
-      </c>
-      <c r="K25" s="42">
-        <v>0</v>
-      </c>
-      <c r="L25" s="42">
+      <c r="F26" s="50"/>
+      <c r="G26" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="40">
+        <v>0</v>
+      </c>
+      <c r="K26" s="42">
+        <v>0</v>
+      </c>
+      <c r="L26" s="42">
         <v>100</v>
       </c>
-      <c r="M25" s="42">
+      <c r="M26" s="42">
         <v>15</v>
       </c>
-      <c r="N25" s="42">
-        <f>(L25-K25)/6</f>
+      <c r="N26" s="42">
+        <f>(L26-K26)/6</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="O25" s="42">
+      <c r="O26" s="42">
         <v>1</v>
       </c>
-      <c r="R25" s="40" t="s">
+      <c r="R26" s="40" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="30" t="s">
+    <row r="27" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="30" t="s">
         <v>673</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E27" s="30" t="s">
         <v>674</v>
       </c>
-      <c r="F26" s="64"/>
-      <c r="G26" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="I26" s="30">
+      <c r="F27" s="64"/>
+      <c r="G27" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="57" t="s">
+    <row r="28" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="57" t="s">
         <v>676</v>
       </c>
-      <c r="E27" s="56" t="s">
+      <c r="E28" s="56" t="s">
         <v>675</v>
       </c>
-      <c r="F27" s="64"/>
-      <c r="G27" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="I27" s="56">
-        <v>0</v>
-      </c>
-      <c r="K27" s="58">
-        <v>0</v>
-      </c>
-      <c r="L27" s="58">
+      <c r="F28" s="64"/>
+      <c r="G28" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="56">
+        <v>0</v>
+      </c>
+      <c r="K28" s="58">
+        <v>0</v>
+      </c>
+      <c r="L28" s="58">
         <v>0.1</v>
       </c>
-      <c r="M27" s="58">
+      <c r="M28" s="58">
         <v>0.05</v>
       </c>
-      <c r="N27" s="58">
-        <f>(L27-K27)/6</f>
+      <c r="N28" s="58">
+        <f>(L28-K28)/6</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="O27" s="58">
+      <c r="O28" s="58">
         <v>0.01</v>
       </c>
-      <c r="R27" s="56" t="s">
+      <c r="R28" s="56" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="30" t="s">
+    <row r="29" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="30" t="s">
         <v>678</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E29" s="30" t="s">
         <v>677</v>
       </c>
-      <c r="F28" s="64"/>
-      <c r="G28" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>680</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>679</v>
-      </c>
-      <c r="F29" s="65"/>
+      <c r="F29" s="64"/>
       <c r="G29" s="30" t="s">
         <v>62</v>
       </c>
@@ -7921,10 +7928,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>69</v>
+        <v>680</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>46</v>
+        <v>679</v>
       </c>
       <c r="F30" s="65"/>
       <c r="G30" s="30" t="s">
@@ -7939,10 +7946,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F31" s="65"/>
       <c r="G31" s="30" t="s">
@@ -7957,132 +7964,123 @@
         <v>21</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F32" s="65"/>
       <c r="G32" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B33" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="65"/>
+      <c r="G33" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="30">
+      <c r="I33" s="30">
         <v>1</v>
       </c>
-      <c r="P32" s="31"/>
-    </row>
-    <row r="33" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="46" t="b">
+      <c r="P33" s="31"/>
+    </row>
+    <row r="34" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B34" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C34" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D34" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E34" s="46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30" t="s">
+    <row r="35" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E35" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="65"/>
-      <c r="G34" s="30" t="s">
+      <c r="F35" s="65"/>
+      <c r="G35" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30" t="s">
+      <c r="H35" s="30"/>
+      <c r="I35" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="30" t="s">
+      <c r="J35" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="Q34" s="39"/>
-    </row>
-    <row r="35" spans="1:18" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B35" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="52" t="s">
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="Q35" s="39"/>
+    </row>
+    <row r="36" spans="1:18" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="52" t="s">
         <v>655</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E36" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="52">
-        <v>0</v>
-      </c>
-      <c r="J35" s="53"/>
-      <c r="K35" s="54">
+      <c r="F36" s="65"/>
+      <c r="G36" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I36" s="52">
+        <v>0</v>
+      </c>
+      <c r="J36" s="53"/>
+      <c r="K36" s="54">
         <v>-40</v>
       </c>
-      <c r="L35" s="54">
+      <c r="L36" s="54">
         <v>40</v>
       </c>
-      <c r="M35" s="54">
-        <v>0</v>
-      </c>
-      <c r="N35" s="54">
-        <f>(L35-K35)/6</f>
+      <c r="M36" s="54">
+        <v>0</v>
+      </c>
+      <c r="N36" s="54">
+        <f>(L36-K36)/6</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="O35" s="54">
+      <c r="O36" s="54">
         <v>1</v>
       </c>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="52" t="s">
+      <c r="Q36" s="55"/>
+      <c r="R36" s="52" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="65"/>
-      <c r="G36" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30">
-        <v>0</v>
-      </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="Q36" s="39"/>
     </row>
     <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
@@ -8090,11 +8088,11 @@
         <v>21</v>
       </c>
       <c r="C37" s="30"/>
-      <c r="D37" s="30" t="s">
-        <v>47</v>
+      <c r="D37" s="44" t="s">
+        <v>45</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F37" s="65"/>
       <c r="G37" s="30" t="s">
@@ -8118,14 +8116,14 @@
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F38" s="65"/>
       <c r="G38" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H38" s="30"/>
       <c r="I38" s="30">
@@ -8145,18 +8143,18 @@
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F39" s="65"/>
       <c r="G39" s="30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H39" s="30"/>
-      <c r="I39" s="30" t="b">
-        <v>1</v>
+      <c r="I39" s="30">
+        <v>0</v>
       </c>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -8172,18 +8170,18 @@
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F40" s="65"/>
       <c r="G40" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H40" s="30"/>
-      <c r="I40" s="30">
-        <v>15</v>
+      <c r="I40" s="30" t="b">
+        <v>1</v>
       </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -8199,18 +8197,18 @@
       </c>
       <c r="C41" s="30"/>
       <c r="D41" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="65"/>
       <c r="G41" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H41" s="30"/>
       <c r="I41" s="30">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -8226,18 +8224,18 @@
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F42" s="65"/>
       <c r="G42" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H42" s="30"/>
       <c r="I42" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
@@ -8246,117 +8244,123 @@
       <c r="O42" s="3"/>
       <c r="Q42" s="39"/>
     </row>
-    <row r="43" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="46" t="b">
+    <row r="43" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="30"/>
+      <c r="B43" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" s="65"/>
+      <c r="G43" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30">
         <v>1</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="Q43" s="39"/>
+    </row>
+    <row r="44" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="B44" s="46" t="s">
         <v>283</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C44" s="46" t="s">
         <v>284</v>
       </c>
-      <c r="D43" s="46" t="s">
+      <c r="D44" s="46" t="s">
         <v>284</v>
       </c>
-      <c r="E43" s="46" t="s">
+      <c r="E44" s="46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B44" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="30" t="s">
+    <row r="45" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="30" t="s">
         <v>371</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E45" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F44" s="65"/>
-      <c r="G44" s="30" t="s">
+      <c r="F45" s="65"/>
+      <c r="G45" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I44" s="30" t="s">
+      <c r="I45" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="30" t="s">
+      <c r="J45" s="30" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="40" t="s">
+    <row r="46" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="40" t="s">
+      <c r="D46" s="40" t="s">
         <v>658</v>
       </c>
-      <c r="E45" s="40" t="s">
+      <c r="E46" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F45" s="50"/>
-      <c r="G45" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H45" s="40" t="s">
+      <c r="F46" s="50"/>
+      <c r="G46" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" s="40" t="s">
         <v>659</v>
       </c>
-      <c r="I45" s="40">
-        <v>0</v>
-      </c>
-      <c r="J45" s="43"/>
-      <c r="K45" s="42">
+      <c r="I46" s="40">
+        <v>0</v>
+      </c>
+      <c r="J46" s="43"/>
+      <c r="K46" s="42">
         <v>-80</v>
       </c>
-      <c r="L45" s="42">
+      <c r="L46" s="42">
         <v>80</v>
       </c>
-      <c r="M45" s="42">
-        <v>0</v>
-      </c>
-      <c r="N45" s="42">
-        <f>(L45-K45)/6</f>
+      <c r="M46" s="42">
+        <v>0</v>
+      </c>
+      <c r="N46" s="42">
+        <f>(L46-K46)/6</f>
         <v>26.666666666666668</v>
       </c>
-      <c r="O45" s="42">
+      <c r="O46" s="42">
         <v>1</v>
       </c>
-      <c r="R45" s="40" t="s">
+      <c r="R46" s="40" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="30" t="s">
+    <row r="47" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="30" t="s">
         <v>660</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="E47" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="65"/>
-      <c r="G46" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H46" s="30" t="s">
-        <v>659</v>
-      </c>
-      <c r="I46" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>661</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" s="64"/>
+      <c r="F47" s="65"/>
       <c r="G47" s="30" t="s">
         <v>62</v>
       </c>
@@ -8372,17 +8376,17 @@
         <v>21</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F48" s="64"/>
       <c r="G48" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I48" s="30">
         <v>0</v>
@@ -8393,16 +8397,19 @@
         <v>21</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F49" s="64"/>
       <c r="G49" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I49" s="30" t="b">
+        <v>63</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>663</v>
+      </c>
+      <c r="I49" s="30">
         <v>0</v>
       </c>
     </row>
@@ -8411,20 +8418,17 @@
         <v>21</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F50" s="64"/>
       <c r="G50" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H50" s="30" t="s">
-        <v>663</v>
-      </c>
-      <c r="I50" s="30">
-        <v>15</v>
+        <v>61</v>
+      </c>
+      <c r="I50" s="30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8432,138 +8436,141 @@
         <v>21</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F51" s="64"/>
       <c r="G51" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H51" s="30" t="s">
+        <v>663</v>
+      </c>
+      <c r="I51" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" s="64"/>
+      <c r="G52" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H52" s="30" t="s">
         <v>659</v>
       </c>
-      <c r="I51" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="30" t="s">
+      <c r="I52" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B53" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="30" t="s">
         <v>667</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="E53" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F52" s="65"/>
-      <c r="G52" s="30" t="s">
+      <c r="F53" s="65"/>
+      <c r="G53" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="H53" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="I52" s="30">
+      <c r="I53" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="46" t="b">
+    <row r="54" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="46" t="s">
+      <c r="B54" s="46" t="s">
         <v>761</v>
       </c>
-      <c r="C53" s="46" t="s">
+      <c r="C54" s="46" t="s">
         <v>762</v>
       </c>
-      <c r="D53" s="46" t="s">
+      <c r="D54" s="46" t="s">
         <v>762</v>
       </c>
-      <c r="E53" s="46" t="s">
+      <c r="E54" s="46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="30" t="s">
+    <row r="55" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="30" t="s">
         <v>342</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="E55" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="65"/>
-      <c r="G54" s="30" t="s">
+      <c r="F55" s="65"/>
+      <c r="G55" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I54" s="51" t="s">
+      <c r="I55" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="J54" s="30" t="s">
+      <c r="J55" s="30" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="55" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="40" t="s">
+    <row r="56" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B56" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D56" s="40" t="s">
         <v>763</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E56" s="40" t="s">
         <v>764</v>
       </c>
-      <c r="F55" s="50"/>
-      <c r="G55" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H55" s="40" t="s">
+      <c r="F56" s="50"/>
+      <c r="G56" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H56" s="40" t="s">
         <v>659</v>
       </c>
-      <c r="I55" s="40">
+      <c r="I56" s="40">
         <v>0.8</v>
       </c>
-      <c r="J55" s="43"/>
-      <c r="K55" s="42">
+      <c r="J56" s="43"/>
+      <c r="K56" s="42">
         <v>0.78</v>
       </c>
-      <c r="L55" s="42">
+      <c r="L56" s="42">
         <v>0.98</v>
       </c>
-      <c r="M55" s="42">
+      <c r="M56" s="42">
         <v>0.8</v>
       </c>
-      <c r="N55" s="42">
-        <f>(L55-K55)/6</f>
+      <c r="N56" s="42">
+        <f>(L56-K56)/6</f>
         <v>3.3333333333333326E-2</v>
       </c>
-      <c r="O55" s="42">
+      <c r="O56" s="42">
         <v>1</v>
       </c>
-      <c r="R55" s="40" t="s">
+      <c r="R56" s="40" t="s">
         <v>654</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>347</v>
-      </c>
-      <c r="E56" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F56" s="31"/>
-      <c r="G56" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I56" s="30" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8571,19 +8578,16 @@
         <v>21</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>660</v>
+        <v>347</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="F57" s="31"/>
       <c r="G57" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H57" s="30" t="s">
-        <v>659</v>
-      </c>
-      <c r="I57" s="30">
+        <v>61</v>
+      </c>
+      <c r="I57" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -8592,10 +8596,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="F58" s="31"/>
       <c r="G58" s="30" t="s">
@@ -8613,37 +8617,40 @@
         <v>21</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F59" s="31"/>
       <c r="G59" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>659</v>
+      </c>
+      <c r="I59" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>662</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F60" s="31"/>
+      <c r="G60" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="H60" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="I59" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B60" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" s="30" t="s">
-        <v>664</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F60" s="65"/>
-      <c r="G60" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I60" s="30" t="b">
+      <c r="I60" s="30">
         <v>0</v>
       </c>
     </row>
@@ -8652,20 +8659,17 @@
         <v>21</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F61" s="65"/>
       <c r="G61" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H61" s="30" t="s">
-        <v>663</v>
-      </c>
-      <c r="I61" s="30">
-        <v>15</v>
+        <v>61</v>
+      </c>
+      <c r="I61" s="30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8673,20 +8677,20 @@
         <v>21</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F62" s="65"/>
       <c r="G62" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="I62" s="30">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8694,117 +8698,120 @@
         <v>21</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F63" s="65"/>
       <c r="G63" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H63" s="30" t="s">
+        <v>659</v>
+      </c>
+      <c r="I63" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B64" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>667</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F64" s="65"/>
+      <c r="G64" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H63" s="30" t="s">
+      <c r="H64" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="I63" s="30">
+      <c r="I64" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="46" t="b">
+    <row r="65" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B65" s="46" t="s">
         <v>768</v>
       </c>
-      <c r="C64" s="46" t="s">
+      <c r="C65" s="46" t="s">
         <v>767</v>
       </c>
-      <c r="D64" s="46" t="s">
+      <c r="D65" s="46" t="s">
         <v>767</v>
       </c>
-      <c r="E64" s="46" t="s">
+      <c r="E65" s="46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B65" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" s="30" t="s">
+    <row r="66" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="30" t="s">
         <v>769</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E66" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="F65" s="65"/>
-      <c r="G65" s="30" t="s">
+      <c r="F66" s="65"/>
+      <c r="G66" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I65" s="51" t="s">
+      <c r="I66" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="J65" s="30" t="s">
+      <c r="J66" s="30" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="66" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B66" s="40" t="s">
+    <row r="67" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B67" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="40" t="s">
+      <c r="D67" s="40" t="s">
         <v>770</v>
       </c>
-      <c r="E66" s="40" t="s">
+      <c r="E67" s="40" t="s">
         <v>771</v>
       </c>
-      <c r="F66" s="50"/>
-      <c r="G66" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H66" s="40" t="s">
+      <c r="F67" s="50"/>
+      <c r="G67" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H67" s="40" t="s">
         <v>659</v>
       </c>
-      <c r="I66" s="40">
+      <c r="I67" s="40">
         <v>4</v>
       </c>
-      <c r="J66" s="43"/>
-      <c r="K66" s="42">
-        <v>2</v>
-      </c>
-      <c r="L66" s="42">
+      <c r="J67" s="43"/>
+      <c r="K67" s="42">
+        <v>2</v>
+      </c>
+      <c r="L67" s="42">
         <v>5</v>
       </c>
-      <c r="M66" s="42">
+      <c r="M67" s="42">
         <v>4</v>
       </c>
-      <c r="N66" s="42">
-        <f>(L66-K66)/6</f>
+      <c r="N67" s="42">
+        <f>(L67-K67)/6</f>
         <v>0.5</v>
       </c>
-      <c r="O66" s="42">
+      <c r="O67" s="42">
         <v>0.25</v>
       </c>
-      <c r="R66" s="40" t="s">
+      <c r="R67" s="40" t="s">
         <v>654</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B67" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>347</v>
-      </c>
-      <c r="E67" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F67" s="65"/>
-      <c r="G67" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I67" s="30" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8812,19 +8819,16 @@
         <v>21</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>660</v>
+        <v>347</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="F68" s="65"/>
       <c r="G68" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H68" s="30" t="s">
-        <v>659</v>
-      </c>
-      <c r="I68" s="30">
+        <v>61</v>
+      </c>
+      <c r="I68" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -8833,10 +8837,10 @@
         <v>21</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="F69" s="65"/>
       <c r="G69" s="30" t="s">
@@ -8854,17 +8858,17 @@
         <v>21</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F70" s="65"/>
       <c r="G70" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I70" s="30">
         <v>0</v>
@@ -8875,16 +8879,19 @@
         <v>21</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F71" s="65"/>
       <c r="G71" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I71" s="30" t="b">
+        <v>63</v>
+      </c>
+      <c r="H71" s="30" t="s">
+        <v>663</v>
+      </c>
+      <c r="I71" s="30">
         <v>0</v>
       </c>
     </row>
@@ -8893,20 +8900,17 @@
         <v>21</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F72" s="65"/>
       <c r="G72" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H72" s="30" t="s">
-        <v>663</v>
-      </c>
-      <c r="I72" s="30">
-        <v>15</v>
+        <v>61</v>
+      </c>
+      <c r="I72" s="30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8914,20 +8918,20 @@
         <v>21</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F73" s="65"/>
       <c r="G73" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="I73" s="30">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8935,99 +8939,79 @@
         <v>21</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F74" s="65"/>
       <c r="G74" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H74" s="30" t="s">
+        <v>659</v>
+      </c>
+      <c r="I74" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B75" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>667</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F75" s="65"/>
+      <c r="G75" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H74" s="30" t="s">
+      <c r="H75" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="I74" s="30">
+      <c r="I75" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="46" t="b">
+    <row r="76" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B75" s="46" t="s">
+      <c r="B76" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="C75" s="46" t="s">
+      <c r="C76" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="D75" s="46" t="s">
+      <c r="D76" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="E75" s="46" t="s">
+      <c r="E76" s="46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B76" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="30" t="s">
+    <row r="77" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B77" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E77" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="F76" s="65"/>
-      <c r="G76" s="30" t="s">
+      <c r="F77" s="65"/>
+      <c r="G77" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I76" s="51" t="s">
+      <c r="I77" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="J76" s="30" t="s">
+      <c r="J77" s="30" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B77" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D77" s="40" t="s">
-        <v>772</v>
-      </c>
-      <c r="E77" s="40" t="s">
-        <v>243</v>
-      </c>
-      <c r="F77" s="50"/>
-      <c r="G77" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H77" s="40" t="s">
-        <v>659</v>
-      </c>
-      <c r="I77" s="40">
-        <v>0</v>
-      </c>
-      <c r="J77" s="43"/>
-      <c r="K77" s="42">
-        <v>-20</v>
-      </c>
-      <c r="L77" s="42">
-        <v>14</v>
-      </c>
-      <c r="M77" s="42">
-        <v>0</v>
-      </c>
-      <c r="N77" s="42">
-        <f>(L77-K77)/6</f>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="O77" s="42">
-        <v>1</v>
-      </c>
-      <c r="R77" s="40" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="78" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9035,10 +9019,10 @@
         <v>22</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E78" s="40" t="s">
-        <v>774</v>
+        <v>243</v>
       </c>
       <c r="F78" s="50"/>
       <c r="G78" s="40" t="s">
@@ -9052,17 +9036,17 @@
       </c>
       <c r="J78" s="43"/>
       <c r="K78" s="42">
-        <v>-25</v>
+        <v>-20</v>
       </c>
       <c r="L78" s="42">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="M78" s="42">
         <v>0</v>
       </c>
       <c r="N78" s="42">
         <f>(L78-K78)/6</f>
-        <v>9.1666666666666661</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="O78" s="42">
         <v>1</v>
@@ -9071,22 +9055,45 @@
         <v>654</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B79" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="30" t="s">
-        <v>347</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F79" s="65"/>
-      <c r="G79" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I79" s="30" t="b">
-        <v>0</v>
+    <row r="79" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B79" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="40" t="s">
+        <v>773</v>
+      </c>
+      <c r="E79" s="40" t="s">
+        <v>774</v>
+      </c>
+      <c r="F79" s="50"/>
+      <c r="G79" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H79" s="40" t="s">
+        <v>659</v>
+      </c>
+      <c r="I79" s="40">
+        <v>0</v>
+      </c>
+      <c r="J79" s="43"/>
+      <c r="K79" s="42">
+        <v>-25</v>
+      </c>
+      <c r="L79" s="42">
+        <v>30</v>
+      </c>
+      <c r="M79" s="42">
+        <v>0</v>
+      </c>
+      <c r="N79" s="42">
+        <f>(L79-K79)/6</f>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="O79" s="42">
+        <v>1</v>
+      </c>
+      <c r="R79" s="40" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9094,19 +9101,16 @@
         <v>21</v>
       </c>
       <c r="D80" s="30" t="s">
-        <v>660</v>
+        <v>347</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="F80" s="65"/>
       <c r="G80" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H80" s="30" t="s">
-        <v>659</v>
-      </c>
-      <c r="I80" s="30">
+        <v>61</v>
+      </c>
+      <c r="I80" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -9115,10 +9119,10 @@
         <v>21</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="F81" s="65"/>
       <c r="G81" s="30" t="s">
@@ -9136,37 +9140,40 @@
         <v>21</v>
       </c>
       <c r="D82" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F82" s="65"/>
       <c r="G82" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H82" s="30" t="s">
+        <v>659</v>
+      </c>
+      <c r="I82" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B83" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>662</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F83" s="65"/>
+      <c r="G83" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H82" s="30" t="s">
+      <c r="H83" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="I82" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="30" t="s">
-        <v>664</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F83" s="64"/>
-      <c r="G83" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I83" s="30" t="b">
+      <c r="I83" s="30">
         <v>0</v>
       </c>
     </row>
@@ -9175,20 +9182,17 @@
         <v>21</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F84" s="64"/>
       <c r="G84" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H84" s="30" t="s">
-        <v>663</v>
-      </c>
-      <c r="I84" s="30">
-        <v>15</v>
+        <v>61</v>
+      </c>
+      <c r="I84" s="30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -9196,20 +9200,20 @@
         <v>21</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F85" s="64"/>
       <c r="G85" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="I85" s="30">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -9217,78 +9221,58 @@
         <v>21</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F86" s="64"/>
       <c r="G86" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H86" s="30" t="s">
+        <v>659</v>
+      </c>
+      <c r="I86" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>667</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" s="64"/>
+      <c r="G87" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H86" s="30" t="s">
+      <c r="H87" s="30" t="s">
         <v>663</v>
       </c>
-      <c r="I86" s="30">
+      <c r="I87" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="46" t="b">
+    <row r="88" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B87" s="46" t="s">
+      <c r="B88" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="C87" s="46" t="s">
+      <c r="C88" s="46" t="s">
         <v>668</v>
       </c>
-      <c r="D87" s="46" t="s">
+      <c r="D88" s="46" t="s">
         <v>668</v>
       </c>
-      <c r="E87" s="46" t="s">
+      <c r="E88" s="46" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B88" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D88" s="40" t="s">
-        <v>669</v>
-      </c>
-      <c r="E88" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="F88" s="50"/>
-      <c r="G88" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H88" s="40" t="s">
-        <v>670</v>
-      </c>
-      <c r="I88" s="40">
-        <v>0</v>
-      </c>
-      <c r="J88" s="43"/>
-      <c r="K88" s="42">
-        <v>-6</v>
-      </c>
-      <c r="L88" s="42">
-        <v>2</v>
-      </c>
-      <c r="M88" s="42">
-        <v>0</v>
-      </c>
-      <c r="N88" s="42">
-        <f>(L88-K88)/6</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="O88" s="42">
-        <v>1</v>
-      </c>
-      <c r="R88" s="40" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="89" spans="1:20" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9296,10 +9280,10 @@
         <v>22</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E89" s="40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F89" s="50"/>
       <c r="G89" s="40" t="s">
@@ -9316,14 +9300,14 @@
         <v>-6</v>
       </c>
       <c r="L89" s="42">
-        <v>3.9</v>
+        <v>2</v>
       </c>
       <c r="M89" s="42">
         <v>0</v>
       </c>
       <c r="N89" s="42">
         <f>(L89-K89)/6</f>
-        <v>1.6500000000000001</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="O89" s="42">
         <v>1</v>
@@ -9332,113 +9316,111 @@
         <v>654</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B90" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="31" t="s">
+    <row r="90" spans="1:20" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B90" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" s="40" t="s">
+        <v>671</v>
+      </c>
+      <c r="E90" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="F90" s="50"/>
+      <c r="G90" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H90" s="40" t="s">
+        <v>670</v>
+      </c>
+      <c r="I90" s="40">
+        <v>0</v>
+      </c>
+      <c r="J90" s="43"/>
+      <c r="K90" s="42">
+        <v>-6</v>
+      </c>
+      <c r="L90" s="42">
+        <v>3.9</v>
+      </c>
+      <c r="M90" s="42">
+        <v>0</v>
+      </c>
+      <c r="N90" s="42">
+        <f>(L90-K90)/6</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="O90" s="42">
+        <v>1</v>
+      </c>
+      <c r="R90" s="40" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B91" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D91" s="31" t="s">
         <v>672</v>
       </c>
-      <c r="E90" s="31" t="s">
+      <c r="E91" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="F90" s="64"/>
-      <c r="G90" s="31" t="s">
+      <c r="F91" s="64"/>
+      <c r="G91" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I90" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
-    </row>
-    <row r="91" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="49" t="b">
+      <c r="I91" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+    </row>
+    <row r="92" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B91" s="49" t="s">
+      <c r="B92" s="49" t="s">
         <v>743</v>
       </c>
-      <c r="C91" s="49" t="s">
+      <c r="C92" s="49" t="s">
         <v>744</v>
       </c>
-      <c r="D91" s="49" t="s">
+      <c r="D92" s="49" t="s">
         <v>744</v>
       </c>
-      <c r="E91" s="46" t="s">
+      <c r="E92" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="F91" s="46"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="49"/>
-      <c r="J91" s="49"/>
-      <c r="K91" s="49"/>
-      <c r="L91" s="49"/>
-      <c r="M91" s="46"/>
-      <c r="N91" s="46"/>
-      <c r="O91" s="46"/>
-      <c r="P91" s="46"/>
-      <c r="Q91" s="46"/>
-      <c r="R91" s="46"/>
-    </row>
-    <row r="92" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="40"/>
-      <c r="B92" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50" t="s">
-        <v>737</v>
-      </c>
-      <c r="E92" s="50" t="s">
-        <v>738</v>
-      </c>
-      <c r="F92" s="50"/>
-      <c r="G92" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="H92" s="50"/>
-      <c r="I92" s="50">
-        <v>1</v>
-      </c>
-      <c r="J92" s="50"/>
-      <c r="K92" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="L92" s="50">
-        <v>4.5</v>
-      </c>
-      <c r="M92" s="42">
-        <v>1.75</v>
-      </c>
-      <c r="N92" s="40">
-        <f>1.5/6</f>
-        <v>0.25</v>
-      </c>
-      <c r="O92" s="50">
-        <v>0.1</v>
-      </c>
-      <c r="P92" s="40"/>
-      <c r="Q92" s="40"/>
-      <c r="R92" s="40" t="s">
-        <v>654</v>
-      </c>
+      <c r="F92" s="46"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="49"/>
+      <c r="L92" s="49"/>
+      <c r="M92" s="46"/>
+      <c r="N92" s="46"/>
+      <c r="O92" s="46"/>
+      <c r="P92" s="46"/>
+      <c r="Q92" s="46"/>
+      <c r="R92" s="46"/>
     </row>
     <row r="93" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="50"/>
+      <c r="A93" s="40"/>
       <c r="B93" s="50" t="s">
         <v>22</v>
       </c>
       <c r="C93" s="50"/>
       <c r="D93" s="50" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E93" s="50" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F93" s="50"/>
       <c r="G93" s="50" t="s">
@@ -9450,7 +9432,7 @@
       </c>
       <c r="J93" s="50"/>
       <c r="K93" s="50">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="L93" s="50">
         <v>4.5</v>
@@ -9458,7 +9440,8 @@
       <c r="M93" s="42">
         <v>1.75</v>
       </c>
-      <c r="N93" s="50">
+      <c r="N93" s="40">
+        <f>1.5/6</f>
         <v>0.25</v>
       </c>
       <c r="O93" s="50">
@@ -9477,10 +9460,10 @@
       </c>
       <c r="C94" s="50"/>
       <c r="D94" s="50" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E94" s="50" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F94" s="50"/>
       <c r="G94" s="50" t="s">
@@ -9492,111 +9475,110 @@
       </c>
       <c r="J94" s="50"/>
       <c r="K94" s="50">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="L94" s="50">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="M94" s="42">
         <v>1.75</v>
       </c>
-      <c r="N94" s="42">
+      <c r="N94" s="50">
         <v>0.25</v>
       </c>
-      <c r="O94" s="42">
+      <c r="O94" s="50">
         <v>0.1</v>
       </c>
-      <c r="P94" s="42"/>
-      <c r="Q94" s="42"/>
+      <c r="P94" s="40"/>
+      <c r="Q94" s="40"/>
       <c r="R94" s="40" t="s">
         <v>654</v>
       </c>
-      <c r="T94" s="31"/>
-    </row>
-    <row r="95" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="49" t="b">
+    </row>
+    <row r="95" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="50"/>
+      <c r="B95" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="50"/>
+      <c r="D95" s="50" t="s">
+        <v>741</v>
+      </c>
+      <c r="E95" s="50" t="s">
+        <v>742</v>
+      </c>
+      <c r="F95" s="50"/>
+      <c r="G95" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H95" s="50"/>
+      <c r="I95" s="50">
         <v>1</v>
       </c>
-      <c r="B95" s="49" t="s">
+      <c r="J95" s="50"/>
+      <c r="K95" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L95" s="50">
+        <v>3</v>
+      </c>
+      <c r="M95" s="42">
+        <v>1.75</v>
+      </c>
+      <c r="N95" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="O95" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="P95" s="42"/>
+      <c r="Q95" s="42"/>
+      <c r="R95" s="40" t="s">
+        <v>654</v>
+      </c>
+      <c r="T95" s="31"/>
+    </row>
+    <row r="96" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B96" s="49" t="s">
         <v>745</v>
       </c>
-      <c r="C95" s="49" t="s">
+      <c r="C96" s="49" t="s">
         <v>746</v>
       </c>
-      <c r="D95" s="49" t="s">
+      <c r="D96" s="49" t="s">
         <v>746</v>
       </c>
-      <c r="E95" s="46" t="s">
+      <c r="E96" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="F95" s="46"/>
-      <c r="G95" s="49"/>
-      <c r="H95" s="49"/>
-      <c r="I95" s="49"/>
-      <c r="J95" s="49"/>
-      <c r="K95" s="49"/>
-      <c r="L95" s="49"/>
-      <c r="M95" s="46"/>
-      <c r="N95" s="46"/>
-      <c r="O95" s="46"/>
-      <c r="P95" s="46"/>
-      <c r="Q95" s="46"/>
-      <c r="R95" s="46"/>
-    </row>
-    <row r="96" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="40"/>
-      <c r="B96" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50" t="s">
-        <v>747</v>
-      </c>
-      <c r="E96" s="50" t="s">
-        <v>738</v>
-      </c>
-      <c r="F96" s="50"/>
-      <c r="G96" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="H96" s="50"/>
-      <c r="I96" s="50">
-        <v>1</v>
-      </c>
-      <c r="J96" s="50"/>
-      <c r="K96" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="L96" s="50">
-        <v>4</v>
-      </c>
-      <c r="M96" s="42">
-        <v>1.75</v>
-      </c>
-      <c r="N96" s="40">
-        <f>1.5/6</f>
-        <v>0.25</v>
-      </c>
-      <c r="O96" s="50">
-        <v>0.1</v>
-      </c>
-      <c r="P96" s="40"/>
-      <c r="Q96" s="40"/>
-      <c r="R96" s="40" t="s">
-        <v>654</v>
-      </c>
+      <c r="F96" s="46"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="49"/>
+      <c r="I96" s="49"/>
+      <c r="J96" s="49"/>
+      <c r="K96" s="49"/>
+      <c r="L96" s="49"/>
+      <c r="M96" s="46"/>
+      <c r="N96" s="46"/>
+      <c r="O96" s="46"/>
+      <c r="P96" s="46"/>
+      <c r="Q96" s="46"/>
+      <c r="R96" s="46"/>
     </row>
     <row r="97" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="50"/>
+      <c r="A97" s="40"/>
       <c r="B97" s="50" t="s">
         <v>22</v>
       </c>
       <c r="C97" s="50"/>
       <c r="D97" s="50" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E97" s="50" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F97" s="50"/>
       <c r="G97" s="50" t="s">
@@ -9616,7 +9598,8 @@
       <c r="M97" s="42">
         <v>1.75</v>
       </c>
-      <c r="N97" s="50">
+      <c r="N97" s="40">
+        <f>1.5/6</f>
         <v>0.25</v>
       </c>
       <c r="O97" s="50">
@@ -9635,10 +9618,10 @@
       </c>
       <c r="C98" s="50"/>
       <c r="D98" s="50" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E98" s="50" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F98" s="50"/>
       <c r="G98" s="50" t="s">
@@ -9653,159 +9636,196 @@
         <v>0.5</v>
       </c>
       <c r="L98" s="50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M98" s="42">
         <v>1.75</v>
       </c>
-      <c r="N98" s="42">
+      <c r="N98" s="50">
         <v>0.25</v>
       </c>
-      <c r="O98" s="42">
+      <c r="O98" s="50">
         <v>0.1</v>
       </c>
-      <c r="P98" s="42"/>
-      <c r="Q98" s="42"/>
+      <c r="P98" s="40"/>
+      <c r="Q98" s="40"/>
       <c r="R98" s="40" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="99" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="46" t="b">
+    <row r="99" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="50"/>
+      <c r="B99" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50" t="s">
+        <v>749</v>
+      </c>
+      <c r="E99" s="50" t="s">
+        <v>742</v>
+      </c>
+      <c r="F99" s="50"/>
+      <c r="G99" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H99" s="50"/>
+      <c r="I99" s="50">
         <v>1</v>
       </c>
-      <c r="B99" s="46" t="s">
+      <c r="J99" s="50"/>
+      <c r="K99" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L99" s="50">
+        <v>3</v>
+      </c>
+      <c r="M99" s="42">
+        <v>1.75</v>
+      </c>
+      <c r="N99" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="O99" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="P99" s="42"/>
+      <c r="Q99" s="42"/>
+      <c r="R99" s="40" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="B100" s="46" t="s">
         <v>776</v>
       </c>
-      <c r="C99" s="46" t="s">
+      <c r="C100" s="46" t="s">
         <v>775</v>
       </c>
-      <c r="D99" s="46" t="s">
+      <c r="D100" s="46" t="s">
         <v>775</v>
       </c>
-      <c r="E99" s="46" t="s">
+      <c r="E100" s="46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D100" s="56" t="s">
+    <row r="101" spans="1:18" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="56" t="s">
         <v>779</v>
       </c>
-      <c r="E100" s="56" t="s">
+      <c r="E101" s="56" t="s">
         <v>777</v>
       </c>
-      <c r="F100" s="64"/>
-      <c r="G100" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="H100" s="56" t="s">
+      <c r="F101" s="64"/>
+      <c r="G101" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="H101" s="56" t="s">
         <v>659</v>
       </c>
-      <c r="I100" s="56">
+      <c r="I101" s="56">
         <v>1</v>
       </c>
-      <c r="J100" s="59"/>
-      <c r="K100" s="58">
+      <c r="J101" s="59"/>
+      <c r="K101" s="58">
         <v>0.9</v>
       </c>
-      <c r="L100" s="58">
+      <c r="L101" s="58">
         <v>1</v>
       </c>
-      <c r="M100" s="58">
+      <c r="M101" s="58">
         <v>0.95</v>
       </c>
-      <c r="N100" s="58">
-        <f>(L100-K100)/6</f>
+      <c r="N101" s="58">
+        <f>(L101-K101)/6</f>
         <v>1.6666666666666663E-2</v>
       </c>
-      <c r="O100" s="58">
+      <c r="O101" s="58">
         <v>0.1</v>
       </c>
-      <c r="R100" s="56" t="s">
+      <c r="R101" s="56" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="101" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B101" s="40" t="s">
+    <row r="102" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B102" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D101" s="40" t="s">
+      <c r="D102" s="40" t="s">
         <v>780</v>
       </c>
-      <c r="E101" s="40" t="s">
+      <c r="E102" s="40" t="s">
         <v>778</v>
       </c>
-      <c r="F101" s="50"/>
-      <c r="G101" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H101" s="40" t="s">
+      <c r="F102" s="50"/>
+      <c r="G102" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H102" s="40" t="s">
         <v>659</v>
       </c>
-      <c r="I101" s="40">
+      <c r="I102" s="40">
         <v>1450</v>
       </c>
-      <c r="J101" s="43"/>
-      <c r="K101" s="42">
-        <v>0</v>
-      </c>
-      <c r="L101" s="42">
+      <c r="J102" s="43"/>
+      <c r="K102" s="42">
+        <v>0</v>
+      </c>
+      <c r="L102" s="42">
         <v>3000</v>
       </c>
-      <c r="M101" s="42">
+      <c r="M102" s="42">
         <v>1450</v>
       </c>
-      <c r="N101" s="42">
-        <f>(L101-K101)/6</f>
+      <c r="N102" s="42">
+        <f>(L102-K102)/6</f>
         <v>500</v>
       </c>
-      <c r="O101" s="42">
+      <c r="O102" s="42">
         <v>50</v>
       </c>
-      <c r="R101" s="40" t="s">
+      <c r="R102" s="40" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A102" s="37" t="b">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A103" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B102" s="37" t="s">
+      <c r="B103" s="37" t="s">
         <v>750</v>
       </c>
-      <c r="C102" s="37" t="s">
+      <c r="C103" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="D102" s="37" t="s">
+      <c r="D103" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="E102" s="37" t="s">
+      <c r="E103" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="F102" s="37"/>
-      <c r="G102" s="37"/>
-      <c r="H102" s="38"/>
-      <c r="I102" s="38"/>
-      <c r="J102" s="37"/>
-      <c r="K102" s="37"/>
-      <c r="L102" s="37"/>
-      <c r="M102" s="37"/>
-      <c r="N102" s="37"/>
-      <c r="O102" s="37"/>
-      <c r="P102" s="37"/>
-      <c r="Q102" s="37"/>
-      <c r="R102" s="37"/>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F103" s="64"/>
-      <c r="I103" s="31"/>
-      <c r="J103" s="31"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="38"/>
+      <c r="I103" s="38"/>
+      <c r="J103" s="37"/>
+      <c r="K103" s="37"/>
+      <c r="L103" s="37"/>
+      <c r="M103" s="37"/>
+      <c r="N103" s="37"/>
+      <c r="O103" s="37"/>
+      <c r="P103" s="37"/>
+      <c r="Q103" s="37"/>
+      <c r="R103" s="37"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F104" s="47"/>
+      <c r="F104" s="64"/>
       <c r="I104" s="31"/>
       <c r="J104" s="31"/>
     </row>
@@ -9845,6 +9865,7 @@
       <c r="J111" s="31"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="F112" s="47"/>
       <c r="I112" s="31"/>
       <c r="J112" s="31"/>
     </row>
@@ -10196,8 +10217,12 @@
       <c r="I199" s="31"/>
       <c r="J199" s="31"/>
     </row>
+    <row r="200" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I200" s="31"/>
+      <c r="J200" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:AA126"/>
+  <autoFilter ref="A2:AA127"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Add PSO spreadsheet for Calibration bump server version in calibration examples
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2424,9 +2424,6 @@
     <t>default</t>
   </si>
   <si>
-    <t>1.12.4</t>
-  </si>
-  <si>
     <t>AddMonthlyJSONUtilityDataElectric</t>
   </si>
   <si>
@@ -2503,6 +2500,9 @@
   </si>
   <si>
     <t>set_runperiod</t>
+  </si>
+  <si>
+    <t>1.12.5</t>
   </si>
 </sst>
 </file>
@@ -6801,7 +6801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6860,7 +6860,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>794</v>
+        <v>820</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -7234,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
@@ -7399,13 +7399,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
+        <v>794</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>795</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>796</v>
-      </c>
       <c r="D4" s="37" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>66</v>
@@ -7418,17 +7418,17 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>797</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>798</v>
       </c>
       <c r="F5" s="64"/>
       <c r="G5" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7437,7 +7437,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>164</v>
@@ -7447,7 +7447,7 @@
         <v>732</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7456,17 +7456,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
+        <v>801</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>802</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>803</v>
       </c>
       <c r="F7" s="64"/>
       <c r="G7" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7475,10 +7475,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>805</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>806</v>
       </c>
       <c r="F8" s="64"/>
       <c r="G8" s="31" t="s">
@@ -7494,17 +7494,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
+        <v>806</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>807</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>808</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="J9" s="31"/>
     </row>
@@ -7551,17 +7551,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
+        <v>809</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>810</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>811</v>
       </c>
       <c r="F12" s="64"/>
       <c r="G12" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I12" s="48" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="J12" s="31"/>
     </row>
@@ -7570,17 +7570,17 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
+        <v>818</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>819</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>820</v>
       </c>
       <c r="F13" s="64"/>
       <c r="G13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="J13" s="31"/>
     </row>
@@ -7589,13 +7589,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>66</v>
@@ -7608,17 +7608,17 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="E15" s="31" t="s">
         <v>797</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>798</v>
       </c>
       <c r="F15" s="64"/>
       <c r="G15" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -7627,7 +7627,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>164</v>
@@ -7637,7 +7637,7 @@
         <v>732</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="J16" s="31"/>
     </row>
@@ -7646,17 +7646,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
+        <v>801</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>802</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>803</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7665,10 +7665,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="E18" s="31" t="s">
         <v>805</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>806</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="31" t="s">
@@ -7684,17 +7684,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
+        <v>806</v>
+      </c>
+      <c r="E19" s="31" t="s">
         <v>807</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>808</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="J19" s="31"/>
     </row>
@@ -7741,17 +7741,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
+        <v>809</v>
+      </c>
+      <c r="E22" s="31" t="s">
         <v>810</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>811</v>
       </c>
       <c r="F22" s="64"/>
       <c r="G22" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="J22" s="31"/>
     </row>

</xml_diff>

<commit_message>
updating LHS spreadsheet for correct directories
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2391,18 +2391,6 @@
     <t>0.4.2</t>
   </si>
   <si>
-    <t>../ASHRAE_example/lib</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/seeds/SEB4_baseboard.osm</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/weather/SRRL_2013AMY_60min.epw</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/measures</t>
-  </si>
-  <si>
     <t>Parameter Short Display Name</t>
   </si>
   <si>
@@ -2503,6 +2491,18 @@
   </si>
   <si>
     <t>1.12.5</t>
+  </si>
+  <si>
+    <t>../Calibration_example/measures</t>
+  </si>
+  <si>
+    <t>../Calibration_example/weather/SRRL_2013AMY_60min.epw</t>
+  </si>
+  <si>
+    <t>../Calibration_example/seeds/SEB4_baseboard.osm</t>
+  </si>
+  <si>
+    <t>../Calibration_example/lib</t>
   </si>
 </sst>
 </file>
@@ -6801,8 +6801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6849,7 +6849,7 @@
         <v>454</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>455</v>
@@ -6860,7 +6860,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -6871,7 +6871,7 @@
         <v>468</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>470</v>
@@ -6953,7 +6953,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>786</v>
+        <v>817</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>652</v>
@@ -7146,7 +7146,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>785</v>
+        <v>818</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7174,7 +7174,7 @@
         <v>641</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>784</v>
+        <v>819</v>
       </c>
       <c r="E40" s="2"/>
     </row>
@@ -7201,7 +7201,7 @@
         <v>643</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>783</v>
+        <v>820</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7234,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
@@ -7334,7 +7334,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7399,13 +7399,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>66</v>
@@ -7418,17 +7418,17 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F5" s="64"/>
       <c r="G5" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7437,7 +7437,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>164</v>
@@ -7447,7 +7447,7 @@
         <v>732</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7456,17 +7456,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="F7" s="64"/>
       <c r="G7" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7475,10 +7475,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="F8" s="64"/>
       <c r="G8" s="31" t="s">
@@ -7494,17 +7494,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="J9" s="31"/>
     </row>
@@ -7551,17 +7551,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="F12" s="64"/>
       <c r="G12" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I12" s="48" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="J12" s="31"/>
     </row>
@@ -7570,17 +7570,17 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="F13" s="64"/>
       <c r="G13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="J13" s="31"/>
     </row>
@@ -7589,13 +7589,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>66</v>
@@ -7608,17 +7608,17 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F15" s="64"/>
       <c r="G15" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -7627,7 +7627,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>164</v>
@@ -7637,7 +7637,7 @@
         <v>732</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="J16" s="31"/>
     </row>
@@ -7646,17 +7646,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7665,10 +7665,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="31" t="s">
@@ -7684,17 +7684,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="J19" s="31"/>
     </row>
@@ -7741,17 +7741,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="F22" s="64"/>
       <c r="G22" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -10281,7 +10281,7 @@
         <v>457</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>630</v>
@@ -10319,7 +10319,7 @@
         <v>622</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>635</v>
@@ -10417,7 +10417,7 @@
         <v>639</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>634</v>
@@ -10449,7 +10449,7 @@
         <v>640</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>633</v>

</xml_diff>

<commit_message>
add SPEA2 update to OS Server 1.13.4
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2385,9 +2385,6 @@
     <t>Baseboard Nominal Capacity (W)</t>
   </si>
   <si>
-    <t>SEB4 baseboard LHS 2013</t>
-  </si>
-  <si>
     <t>0.4.2</t>
   </si>
   <si>
@@ -2409,9 +2406,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>AddMonthlyJSONUtilityDataElectric</t>
   </si>
   <si>
@@ -2490,9 +2484,6 @@
     <t>set_runperiod</t>
   </si>
   <si>
-    <t>1.12.5</t>
-  </si>
-  <si>
     <t>../Calibration_example/measures</t>
   </si>
   <si>
@@ -2503,6 +2494,15 @@
   </si>
   <si>
     <t>../Calibration_example/lib</t>
+  </si>
+  <si>
+    <t>SEB4 baseboard LHS 2013 184</t>
+  </si>
+  <si>
+    <t>default3</t>
+  </si>
+  <si>
+    <t>1.13.4</t>
   </si>
 </sst>
 </file>
@@ -6801,8 +6801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6838,7 +6838,7 @@
         <v>434</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>435</v>
@@ -6849,7 +6849,7 @@
         <v>454</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>455</v>
@@ -6860,7 +6860,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -6871,7 +6871,7 @@
         <v>468</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>789</v>
+        <v>819</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>470</v>
@@ -6942,7 +6942,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>781</v>
+        <v>818</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>469</v>
@@ -6953,7 +6953,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>652</v>
@@ -7146,7 +7146,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7174,7 +7174,7 @@
         <v>641</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="E40" s="2"/>
     </row>
@@ -7201,7 +7201,7 @@
         <v>643</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7221,7 +7221,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7234,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
@@ -7334,7 +7334,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7399,13 +7399,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>66</v>
@@ -7418,17 +7418,17 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F5" s="64"/>
       <c r="G5" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7437,7 +7437,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>164</v>
@@ -7447,7 +7447,7 @@
         <v>732</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7456,17 +7456,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F7" s="64"/>
       <c r="G7" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7475,10 +7475,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F8" s="64"/>
       <c r="G8" s="31" t="s">
@@ -7494,17 +7494,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="J9" s="31"/>
     </row>
@@ -7551,17 +7551,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F12" s="64"/>
       <c r="G12" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I12" s="48" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="J12" s="31"/>
     </row>
@@ -7570,17 +7570,17 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F13" s="64"/>
       <c r="G13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="J13" s="31"/>
     </row>
@@ -7589,13 +7589,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>66</v>
@@ -7608,17 +7608,17 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F15" s="64"/>
       <c r="G15" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -7627,7 +7627,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>164</v>
@@ -7637,7 +7637,7 @@
         <v>732</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="J16" s="31"/>
     </row>
@@ -7646,17 +7646,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7665,10 +7665,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="31" t="s">
@@ -7684,17 +7684,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="31" t="s">
         <v>732</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="J19" s="31"/>
     </row>
@@ -7741,17 +7741,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F22" s="64"/>
       <c r="G22" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -10281,7 +10281,7 @@
         <v>457</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>630</v>
@@ -10319,7 +10319,7 @@
         <v>622</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>635</v>
@@ -10417,7 +10417,7 @@
         <v>639</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>634</v>
@@ -10449,7 +10449,7 @@
         <v>640</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>633</v>

</xml_diff>

<commit_message>
update spreadsheets to use enhanced calibration report.
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="820">
   <si>
     <t>type</t>
   </si>
@@ -1977,12 +1977,6 @@
     <t>Directory</t>
   </si>
   <si>
-    <t>CalibrationReports</t>
-  </si>
-  <si>
-    <t>Calibration Reports</t>
-  </si>
-  <si>
     <t>Total Electricity Consumption Modeled</t>
   </si>
   <si>
@@ -2010,12 +2004,6 @@
     <t>Lighting Power Reduction</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports.gas_bill_consumption_modeled</t>
-  </si>
-  <si>
     <t>Electric Equipment Power Reduction</t>
   </si>
   <si>
@@ -2202,12 +2190,6 @@
     <t>m2</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports.gas_bill_rmse</t>
-  </si>
-  <si>
     <t>Electric RMSE</t>
   </si>
   <si>
@@ -2217,27 +2199,15 @@
     <t>Electric CVRMSE</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_consumption_cvrmse</t>
-  </si>
-  <si>
     <t>Electric NMBE</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_consumption_nmbe</t>
-  </si>
-  <si>
     <t>Gas CVRMSE</t>
   </si>
   <si>
-    <t>calibration_reports.gas_bill_consumption_cvrmse</t>
-  </si>
-  <si>
     <t>Gas NMBE</t>
   </si>
   <si>
-    <t>calibration_reports.gas_bill_consumption_nmbe</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -2304,27 +2274,15 @@
     <t>Electric CVRMSE within limit</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_cvrmse_within_limit</t>
-  </si>
-  <si>
     <t>Electric NMBE within limit</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_nmbe_within_limit</t>
-  </si>
-  <si>
     <t>Gas CVRMSE within limit</t>
   </si>
   <si>
-    <t>calibration_reports.gas_bill_cvrmse_within_limit</t>
-  </si>
-  <si>
     <t>Gas NMBE within limit</t>
   </si>
   <si>
-    <t>calibration_reports.gas_bill_nmbe_within_limit</t>
-  </si>
-  <si>
     <t>Set Gas Burner Efficiency</t>
   </si>
   <si>
@@ -2499,10 +2457,49 @@
     <t>SEB4 baseboard LHS 2013 184</t>
   </si>
   <si>
-    <t>default3</t>
-  </si>
-  <si>
-    <t>1.13.4</t>
+    <t>CalibrationReportsEnhanced</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.electric_bill_consumption_modeled</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.gas_bill_consumption_modeled</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.electric_bill_rmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.gas_bill_rmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.electric_bill_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.electric_bill_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.gas_bill_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.gas_bill_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.electric_bill_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.electric_bill_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.gas_bill_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced.gas_bill_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>1.14.1</t>
   </si>
 </sst>
 </file>
@@ -6802,7 +6799,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6838,7 +6835,7 @@
         <v>434</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>435</v>
@@ -6849,7 +6846,7 @@
         <v>454</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>455</v>
@@ -6860,7 +6857,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -6871,7 +6868,7 @@
         <v>468</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>470</v>
@@ -6942,7 +6939,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>818</v>
+        <v>804</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>469</v>
@@ -6953,10 +6950,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>814</v>
+        <v>800</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6964,10 +6961,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -7133,7 +7130,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>30</v>
@@ -7146,7 +7143,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>815</v>
+        <v>801</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7160,7 +7157,7 @@
         <v>37</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>447</v>
@@ -7174,7 +7171,7 @@
         <v>641</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>816</v>
+        <v>802</v>
       </c>
       <c r="E40" s="2"/>
     </row>
@@ -7186,7 +7183,7 @@
         <v>33</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7201,7 +7198,7 @@
         <v>643</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>817</v>
+        <v>803</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7236,7 +7233,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7334,7 +7331,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7399,13 +7396,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>66</v>
@@ -7418,17 +7415,17 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>790</v>
+        <v>776</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>791</v>
+        <v>777</v>
       </c>
       <c r="F5" s="64"/>
       <c r="G5" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7437,17 +7434,17 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>164</v>
       </c>
       <c r="F6" s="64"/>
       <c r="G6" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>794</v>
+        <v>780</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7456,17 +7453,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>795</v>
+        <v>781</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>796</v>
+        <v>782</v>
       </c>
       <c r="F7" s="64"/>
       <c r="G7" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>797</v>
+        <v>783</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7475,17 +7472,17 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="F8" s="64"/>
       <c r="G8" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J8" s="31"/>
     </row>
@@ -7494,17 +7491,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>800</v>
+        <v>786</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>801</v>
+        <v>787</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="J9" s="31"/>
     </row>
@@ -7513,17 +7510,17 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>734</v>
+        <v>724</v>
       </c>
       <c r="F10" s="64"/>
       <c r="G10" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I10" s="48" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="J10" s="31"/>
     </row>
@@ -7532,17 +7529,17 @@
         <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>735</v>
+        <v>725</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
       <c r="F11" s="64"/>
       <c r="G11" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I11" s="48" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="J11" s="31"/>
     </row>
@@ -7551,17 +7548,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>803</v>
+        <v>789</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="F12" s="64"/>
       <c r="G12" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I12" s="48" t="s">
-        <v>805</v>
+        <v>791</v>
       </c>
       <c r="J12" s="31"/>
     </row>
@@ -7570,17 +7567,17 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>812</v>
+        <v>798</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>813</v>
+        <v>799</v>
       </c>
       <c r="F13" s="64"/>
       <c r="G13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>805</v>
+        <v>791</v>
       </c>
       <c r="J13" s="31"/>
     </row>
@@ -7589,13 +7586,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>806</v>
+        <v>792</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>66</v>
@@ -7608,17 +7605,17 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>790</v>
+        <v>776</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>791</v>
+        <v>777</v>
       </c>
       <c r="F15" s="64"/>
       <c r="G15" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>807</v>
+        <v>793</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -7627,17 +7624,17 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>164</v>
       </c>
       <c r="F16" s="64"/>
       <c r="G16" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>808</v>
+        <v>794</v>
       </c>
       <c r="J16" s="31"/>
     </row>
@@ -7646,17 +7643,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>795</v>
+        <v>781</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>796</v>
+        <v>782</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>809</v>
+        <v>795</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7665,17 +7662,17 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J18" s="31"/>
     </row>
@@ -7684,17 +7681,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>800</v>
+        <v>786</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>801</v>
+        <v>787</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>810</v>
+        <v>796</v>
       </c>
       <c r="J19" s="31"/>
     </row>
@@ -7703,17 +7700,17 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>734</v>
+        <v>724</v>
       </c>
       <c r="F20" s="64"/>
       <c r="G20" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I20" s="48" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="J20" s="31"/>
     </row>
@@ -7722,17 +7719,17 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>735</v>
+        <v>725</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
       <c r="F21" s="64"/>
       <c r="G21" s="31" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="I21" s="48" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="J21" s="31"/>
     </row>
@@ -7741,17 +7738,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>803</v>
+        <v>789</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="F22" s="64"/>
       <c r="G22" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>811</v>
+        <v>797</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -7760,13 +7757,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>646</v>
+        <v>805</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>645</v>
+        <v>805</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>645</v>
+        <v>805</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>231</v>
@@ -7818,7 +7815,7 @@
         <v>22</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>68</v>
@@ -7847,7 +7844,7 @@
         <v>1</v>
       </c>
       <c r="R26" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7855,10 +7852,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="F27" s="64"/>
       <c r="G27" s="30" t="s">
@@ -7873,10 +7870,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="E28" s="56" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="F28" s="64"/>
       <c r="G28" s="56" t="s">
@@ -7902,7 +7899,7 @@
         <v>0.01</v>
       </c>
       <c r="R28" s="56" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7910,10 +7907,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="F29" s="64"/>
       <c r="G29" s="30" t="s">
@@ -7928,10 +7925,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F30" s="65"/>
       <c r="G30" s="30" t="s">
@@ -8048,7 +8045,7 @@
         <v>21</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E36" s="52" t="s">
         <v>44</v>
@@ -8079,7 +8076,7 @@
       </c>
       <c r="Q36" s="55"/>
       <c r="R36" s="52" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -8314,7 +8311,7 @@
         <v>22</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="E46" s="40" t="s">
         <v>286</v>
@@ -8324,7 +8321,7 @@
         <v>62</v>
       </c>
       <c r="H46" s="40" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I46" s="40">
         <v>0</v>
@@ -8347,7 +8344,7 @@
         <v>1</v>
       </c>
       <c r="R46" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8355,7 +8352,7 @@
         <v>21</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="E47" s="30" t="s">
         <v>46</v>
@@ -8365,7 +8362,7 @@
         <v>62</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I47" s="30">
         <v>0</v>
@@ -8376,7 +8373,7 @@
         <v>21</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E48" s="30" t="s">
         <v>48</v>
@@ -8386,7 +8383,7 @@
         <v>62</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I48" s="30">
         <v>0</v>
@@ -8397,7 +8394,7 @@
         <v>21</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E49" s="30" t="s">
         <v>50</v>
@@ -8407,7 +8404,7 @@
         <v>63</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I49" s="30">
         <v>0</v>
@@ -8418,7 +8415,7 @@
         <v>21</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E50" s="30" t="s">
         <v>52</v>
@@ -8436,7 +8433,7 @@
         <v>21</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="E51" s="30" t="s">
         <v>54</v>
@@ -8446,7 +8443,7 @@
         <v>63</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I51" s="30">
         <v>15</v>
@@ -8457,7 +8454,7 @@
         <v>21</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="E52" s="30" t="s">
         <v>56</v>
@@ -8467,7 +8464,7 @@
         <v>62</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I52" s="30">
         <v>0</v>
@@ -8478,7 +8475,7 @@
         <v>21</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E53" s="30" t="s">
         <v>58</v>
@@ -8488,7 +8485,7 @@
         <v>63</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I53" s="30">
         <v>1</v>
@@ -8499,13 +8496,13 @@
         <v>1</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="C54" s="46" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="D54" s="46" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="E54" s="46" t="s">
         <v>66</v>
@@ -8537,17 +8534,17 @@
         <v>22</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
       <c r="E56" s="40" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
       <c r="F56" s="50"/>
       <c r="G56" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H56" s="40" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I56" s="40">
         <v>0.8</v>
@@ -8570,7 +8567,7 @@
         <v>1</v>
       </c>
       <c r="R56" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8596,7 +8593,7 @@
         <v>21</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="E58" s="30" t="s">
         <v>126</v>
@@ -8606,7 +8603,7 @@
         <v>62</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I58" s="30">
         <v>0</v>
@@ -8617,7 +8614,7 @@
         <v>21</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E59" s="30" t="s">
         <v>48</v>
@@ -8627,7 +8624,7 @@
         <v>62</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I59" s="30">
         <v>0</v>
@@ -8638,7 +8635,7 @@
         <v>21</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E60" s="30" t="s">
         <v>50</v>
@@ -8648,7 +8645,7 @@
         <v>63</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I60" s="30">
         <v>0</v>
@@ -8659,7 +8656,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E61" s="30" t="s">
         <v>52</v>
@@ -8677,7 +8674,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="E62" s="30" t="s">
         <v>54</v>
@@ -8687,7 +8684,7 @@
         <v>63</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I62" s="30">
         <v>15</v>
@@ -8698,7 +8695,7 @@
         <v>21</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="E63" s="30" t="s">
         <v>56</v>
@@ -8708,7 +8705,7 @@
         <v>62</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I63" s="30">
         <v>0</v>
@@ -8719,7 +8716,7 @@
         <v>21</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>58</v>
@@ -8729,7 +8726,7 @@
         <v>63</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I64" s="30">
         <v>1</v>
@@ -8740,13 +8737,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>768</v>
+        <v>754</v>
       </c>
       <c r="C65" s="46" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="D65" s="46" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="E65" s="46" t="s">
         <v>66</v>
@@ -8757,7 +8754,7 @@
         <v>21</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="E66" s="30" t="s">
         <v>124</v>
@@ -8778,17 +8775,17 @@
         <v>22</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="E67" s="40" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="F67" s="50"/>
       <c r="G67" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H67" s="40" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I67" s="40">
         <v>4</v>
@@ -8811,7 +8808,7 @@
         <v>0.25</v>
       </c>
       <c r="R67" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8837,7 +8834,7 @@
         <v>21</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="E69" s="30" t="s">
         <v>126</v>
@@ -8847,7 +8844,7 @@
         <v>62</v>
       </c>
       <c r="H69" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I69" s="30">
         <v>0</v>
@@ -8858,7 +8855,7 @@
         <v>21</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E70" s="30" t="s">
         <v>48</v>
@@ -8868,7 +8865,7 @@
         <v>62</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I70" s="30">
         <v>0</v>
@@ -8879,7 +8876,7 @@
         <v>21</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E71" s="30" t="s">
         <v>50</v>
@@ -8889,7 +8886,7 @@
         <v>63</v>
       </c>
       <c r="H71" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I71" s="30">
         <v>0</v>
@@ -8900,7 +8897,7 @@
         <v>21</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E72" s="30" t="s">
         <v>52</v>
@@ -8918,7 +8915,7 @@
         <v>21</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="E73" s="30" t="s">
         <v>54</v>
@@ -8928,7 +8925,7 @@
         <v>63</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I73" s="30">
         <v>15</v>
@@ -8939,7 +8936,7 @@
         <v>21</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="E74" s="30" t="s">
         <v>56</v>
@@ -8949,7 +8946,7 @@
         <v>62</v>
       </c>
       <c r="H74" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I74" s="30">
         <v>0</v>
@@ -8960,7 +8957,7 @@
         <v>21</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E75" s="30" t="s">
         <v>58</v>
@@ -8970,7 +8967,7 @@
         <v>63</v>
       </c>
       <c r="H75" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I75" s="30">
         <v>1</v>
@@ -9019,7 +9016,7 @@
         <v>22</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>243</v>
@@ -9029,7 +9026,7 @@
         <v>62</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I78" s="40">
         <v>0</v>
@@ -9052,7 +9049,7 @@
         <v>1</v>
       </c>
       <c r="R78" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="79" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9060,17 +9057,17 @@
         <v>22</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="E79" s="40" t="s">
-        <v>774</v>
+        <v>760</v>
       </c>
       <c r="F79" s="50"/>
       <c r="G79" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I79" s="40">
         <v>0</v>
@@ -9093,7 +9090,7 @@
         <v>1</v>
       </c>
       <c r="R79" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9119,7 +9116,7 @@
         <v>21</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="E81" s="30" t="s">
         <v>126</v>
@@ -9129,7 +9126,7 @@
         <v>62</v>
       </c>
       <c r="H81" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I81" s="30">
         <v>0</v>
@@ -9140,7 +9137,7 @@
         <v>21</v>
       </c>
       <c r="D82" s="30" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E82" s="30" t="s">
         <v>48</v>
@@ -9150,7 +9147,7 @@
         <v>62</v>
       </c>
       <c r="H82" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I82" s="30">
         <v>0</v>
@@ -9161,7 +9158,7 @@
         <v>21</v>
       </c>
       <c r="D83" s="30" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E83" s="30" t="s">
         <v>50</v>
@@ -9171,7 +9168,7 @@
         <v>63</v>
       </c>
       <c r="H83" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I83" s="30">
         <v>0</v>
@@ -9182,7 +9179,7 @@
         <v>21</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E84" s="30" t="s">
         <v>52</v>
@@ -9200,7 +9197,7 @@
         <v>21</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="E85" s="30" t="s">
         <v>54</v>
@@ -9210,7 +9207,7 @@
         <v>63</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I85" s="30">
         <v>15</v>
@@ -9221,7 +9218,7 @@
         <v>21</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="E86" s="30" t="s">
         <v>56</v>
@@ -9231,7 +9228,7 @@
         <v>62</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I86" s="30">
         <v>0</v>
@@ -9242,7 +9239,7 @@
         <v>21</v>
       </c>
       <c r="D87" s="30" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E87" s="30" t="s">
         <v>58</v>
@@ -9252,7 +9249,7 @@
         <v>63</v>
       </c>
       <c r="H87" s="30" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="I87" s="30">
         <v>1</v>
@@ -9266,10 +9263,10 @@
         <v>185</v>
       </c>
       <c r="C88" s="46" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D88" s="46" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="E88" s="46" t="s">
         <v>66</v>
@@ -9280,7 +9277,7 @@
         <v>22</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="E89" s="40" t="s">
         <v>188</v>
@@ -9290,7 +9287,7 @@
         <v>62</v>
       </c>
       <c r="H89" s="40" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="I89" s="40">
         <v>0</v>
@@ -9313,7 +9310,7 @@
         <v>1</v>
       </c>
       <c r="R89" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="90" spans="1:20" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9321,7 +9318,7 @@
         <v>22</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E90" s="40" t="s">
         <v>190</v>
@@ -9331,7 +9328,7 @@
         <v>62</v>
       </c>
       <c r="H90" s="40" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="I90" s="40">
         <v>0</v>
@@ -9354,7 +9351,7 @@
         <v>1</v>
       </c>
       <c r="R90" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
@@ -9362,7 +9359,7 @@
         <v>21</v>
       </c>
       <c r="D91" s="31" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="E91" s="31" t="s">
         <v>192</v>
@@ -9385,13 +9382,13 @@
         <v>1</v>
       </c>
       <c r="B92" s="49" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="C92" s="49" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="D92" s="49" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="E92" s="46" t="s">
         <v>66</v>
@@ -9417,10 +9414,10 @@
       </c>
       <c r="C93" s="50"/>
       <c r="D93" s="50" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
       <c r="E93" s="50" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="F93" s="50"/>
       <c r="G93" s="50" t="s">
@@ -9450,7 +9447,7 @@
       <c r="P93" s="40"/>
       <c r="Q93" s="40"/>
       <c r="R93" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="94" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9460,10 +9457,10 @@
       </c>
       <c r="C94" s="50"/>
       <c r="D94" s="50" t="s">
-        <v>739</v>
+        <v>729</v>
       </c>
       <c r="E94" s="50" t="s">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="F94" s="50"/>
       <c r="G94" s="50" t="s">
@@ -9492,7 +9489,7 @@
       <c r="P94" s="40"/>
       <c r="Q94" s="40"/>
       <c r="R94" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="95" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9502,10 +9499,10 @@
       </c>
       <c r="C95" s="50"/>
       <c r="D95" s="50" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
       <c r="E95" s="50" t="s">
-        <v>742</v>
+        <v>732</v>
       </c>
       <c r="F95" s="50"/>
       <c r="G95" s="50" t="s">
@@ -9534,7 +9531,7 @@
       <c r="P95" s="42"/>
       <c r="Q95" s="42"/>
       <c r="R95" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="T95" s="31"/>
     </row>
@@ -9543,13 +9540,13 @@
         <v>1</v>
       </c>
       <c r="B96" s="49" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="C96" s="49" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="D96" s="49" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="E96" s="46" t="s">
         <v>66</v>
@@ -9575,10 +9572,10 @@
       </c>
       <c r="C97" s="50"/>
       <c r="D97" s="50" t="s">
-        <v>747</v>
+        <v>737</v>
       </c>
       <c r="E97" s="50" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="F97" s="50"/>
       <c r="G97" s="50" t="s">
@@ -9608,7 +9605,7 @@
       <c r="P97" s="40"/>
       <c r="Q97" s="40"/>
       <c r="R97" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9618,10 +9615,10 @@
       </c>
       <c r="C98" s="50"/>
       <c r="D98" s="50" t="s">
-        <v>748</v>
+        <v>738</v>
       </c>
       <c r="E98" s="50" t="s">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="F98" s="50"/>
       <c r="G98" s="50" t="s">
@@ -9650,7 +9647,7 @@
       <c r="P98" s="40"/>
       <c r="Q98" s="40"/>
       <c r="R98" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9660,10 +9657,10 @@
       </c>
       <c r="C99" s="50"/>
       <c r="D99" s="50" t="s">
-        <v>749</v>
+        <v>739</v>
       </c>
       <c r="E99" s="50" t="s">
-        <v>742</v>
+        <v>732</v>
       </c>
       <c r="F99" s="50"/>
       <c r="G99" s="50" t="s">
@@ -9692,7 +9689,7 @@
       <c r="P99" s="42"/>
       <c r="Q99" s="42"/>
       <c r="R99" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9700,13 +9697,13 @@
         <v>1</v>
       </c>
       <c r="B100" s="46" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
       <c r="C100" s="46" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="D100" s="46" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="E100" s="46" t="s">
         <v>66</v>
@@ -9717,17 +9714,17 @@
         <v>21</v>
       </c>
       <c r="D101" s="56" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="E101" s="56" t="s">
-        <v>777</v>
+        <v>763</v>
       </c>
       <c r="F101" s="64"/>
       <c r="G101" s="56" t="s">
         <v>62</v>
       </c>
       <c r="H101" s="56" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I101" s="56">
         <v>1</v>
@@ -9750,7 +9747,7 @@
         <v>0.1</v>
       </c>
       <c r="R101" s="56" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9758,17 +9755,17 @@
         <v>22</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="E102" s="40" t="s">
-        <v>778</v>
+        <v>764</v>
       </c>
       <c r="F102" s="50"/>
       <c r="G102" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H102" s="40" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I102" s="40">
         <v>1450</v>
@@ -9791,7 +9788,7 @@
         <v>50</v>
       </c>
       <c r="R102" s="40" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -9799,13 +9796,13 @@
         <v>1</v>
       </c>
       <c r="B103" s="37" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="C103" s="37" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="D103" s="37" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="E103" s="37" t="s">
         <v>231</v>
@@ -10241,8 +10238,8 @@
   <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6:B7"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10281,7 +10278,7 @@
         <v>457</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>783</v>
+        <v>769</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>630</v>
@@ -10319,7 +10316,7 @@
         <v>622</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>784</v>
+        <v>770</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>635</v>
@@ -10417,7 +10414,7 @@
         <v>639</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>634</v>
@@ -10449,7 +10446,7 @@
         <v>640</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>786</v>
+        <v>772</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>633</v>
@@ -10478,12 +10475,12 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>466</v>
@@ -10507,12 +10504,12 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>466</v>
@@ -10536,12 +10533,12 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>466</v>
@@ -10564,12 +10561,12 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E11" s="30" t="s">
         <v>466</v>
@@ -10592,12 +10589,12 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>466</v>
@@ -10620,12 +10617,12 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>466</v>
@@ -10648,12 +10645,12 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="30"/>
       <c r="D14" s="30" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>466</v>
@@ -10677,12 +10674,12 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>466</v>
@@ -10706,12 +10703,12 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>466</v>
@@ -10735,12 +10732,12 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>466</v>
@@ -10764,12 +10761,12 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>466</v>
@@ -10793,12 +10790,12 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>466</v>
@@ -10822,12 +10819,12 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>466</v>
@@ -10851,12 +10848,12 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="E21" s="30" t="s">
         <v>466</v>
@@ -10880,15 +10877,15 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="30"/>
       <c r="D22" s="30" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>62</v>
@@ -10909,15 +10906,15 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>62</v>
@@ -10938,15 +10935,15 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>62</v>
@@ -10967,15 +10964,15 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B25" s="47"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>62</v>
@@ -10996,15 +10993,15 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30" t="s">
-        <v>656</v>
+        <v>806</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>62</v>
@@ -11025,15 +11022,15 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30" t="s">
-        <v>657</v>
+        <v>807</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>62</v>
@@ -11054,15 +11051,15 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30" t="s">
-        <v>720</v>
+        <v>808</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>62</v>
@@ -11082,15 +11079,15 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30" t="s">
-        <v>721</v>
+        <v>809</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>62</v>
@@ -11110,21 +11107,21 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
       <c r="D30" s="30" t="s">
-        <v>725</v>
+        <v>810</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G30" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="30" t="b">
         <v>1</v>
@@ -11138,21 +11135,21 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
-        <v>726</v>
+        <v>719</v>
       </c>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30" t="s">
-        <v>727</v>
+        <v>811</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G31" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="30" t="b">
         <v>1</v>
@@ -11166,21 +11163,21 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30" t="s">
-        <v>729</v>
+        <v>812</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G32" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="30" t="b">
         <v>1</v>
@@ -11194,21 +11191,21 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30" t="s">
-        <v>731</v>
+        <v>813</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G33" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="30" t="b">
         <v>1</v>
@@ -11222,19 +11219,19 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
-        <v>753</v>
+        <v>743</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
       <c r="D34" s="30" t="s">
-        <v>754</v>
+        <v>814</v>
       </c>
       <c r="E34" s="30"/>
       <c r="F34" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G34" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="30" t="b">
         <v>1</v>
@@ -11245,19 +11242,19 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
-        <v>755</v>
+        <v>744</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="30" t="s">
-        <v>756</v>
+        <v>815</v>
       </c>
       <c r="E35" s="30"/>
       <c r="F35" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G35" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="30" t="b">
         <v>1</v>
@@ -11268,19 +11265,19 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
-        <v>757</v>
+        <v>745</v>
       </c>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="30" t="s">
-        <v>758</v>
+        <v>816</v>
       </c>
       <c r="E36" s="30"/>
       <c r="F36" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G36" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="30" t="b">
         <v>1</v>
@@ -11291,17 +11288,17 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>759</v>
+        <v>746</v>
       </c>
       <c r="B37" s="30"/>
       <c r="D37" s="30" t="s">
-        <v>760</v>
+        <v>817</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G37" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="30" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
fixing typo in calibration reports enhanced display name
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="821">
   <si>
     <t>type</t>
   </si>
@@ -2500,6 +2500,9 @@
   </si>
   <si>
     <t>1.14.1</t>
+  </si>
+  <si>
+    <t>Calibration Reports Enhanced</t>
   </si>
 </sst>
 </file>
@@ -6798,7 +6801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -7231,9 +7234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7757,7 +7760,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>805</v>
+        <v>820</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>805</v>

</xml_diff>

<commit_message>
bump server version to 1.14.4 which has calibration report fix
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2499,10 +2499,10 @@
     <t>default</t>
   </si>
   <si>
-    <t>1.14.1</t>
-  </si>
-  <si>
     <t>Calibration Reports Enhanced</t>
+  </si>
+  <si>
+    <t>1.14.4</t>
   </si>
 </sst>
 </file>
@@ -6801,8 +6801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6860,7 +6860,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -7234,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
@@ -7760,7 +7760,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>805</v>

</xml_diff>

<commit_message>
remove _uncertain from distribution types
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -1998,9 +1998,6 @@
     <t>Files to include (relative to this spreadsheet or absolute path). If a directory then it will include all subfolders and files</t>
   </si>
   <si>
-    <t>uniform_uncertain</t>
-  </si>
-  <si>
     <t>Lighting Power Reduction</t>
   </si>
   <si>
@@ -2503,6 +2500,9 @@
   </si>
   <si>
     <t>1.14.4</t>
+  </si>
+  <si>
+    <t>uniform</t>
   </si>
 </sst>
 </file>
@@ -6801,7 +6801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6838,7 +6838,7 @@
         <v>434</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>435</v>
@@ -6849,7 +6849,7 @@
         <v>454</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>455</v>
@@ -6860,7 +6860,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>612</v>
@@ -6871,7 +6871,7 @@
         <v>468</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>470</v>
@@ -6942,7 +6942,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>469</v>
@@ -6953,7 +6953,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>650</v>
@@ -6964,7 +6964,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>650</v>
@@ -7146,7 +7146,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7174,7 +7174,7 @@
         <v>641</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E40" s="2"/>
     </row>
@@ -7201,7 +7201,7 @@
         <v>643</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7234,9 +7234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R105" sqref="R105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7334,7 +7334,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7399,13 +7399,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
+        <v>773</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>774</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>775</v>
-      </c>
       <c r="D4" s="37" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>66</v>
@@ -7418,17 +7418,17 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>775</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>776</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>777</v>
       </c>
       <c r="F5" s="64"/>
       <c r="G5" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7437,17 +7437,17 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>164</v>
       </c>
       <c r="F6" s="64"/>
       <c r="G6" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7456,17 +7456,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
+        <v>780</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>781</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>782</v>
       </c>
       <c r="F7" s="64"/>
       <c r="G7" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7475,14 +7475,14 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
+        <v>783</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>784</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>785</v>
       </c>
       <c r="F8" s="64"/>
       <c r="G8" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I8" s="31" t="s">
         <v>646</v>
@@ -7494,17 +7494,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
+        <v>785</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>786</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>787</v>
       </c>
       <c r="F9" s="64"/>
       <c r="G9" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="J9" s="31"/>
     </row>
@@ -7513,17 +7513,17 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
+        <v>722</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>723</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>724</v>
       </c>
       <c r="F10" s="64"/>
       <c r="G10" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I10" s="48" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J10" s="31"/>
     </row>
@@ -7532,17 +7532,17 @@
         <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
+        <v>724</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>725</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>726</v>
       </c>
       <c r="F11" s="64"/>
       <c r="G11" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I11" s="48" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J11" s="31"/>
     </row>
@@ -7551,17 +7551,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>789</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>790</v>
       </c>
       <c r="F12" s="64"/>
       <c r="G12" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I12" s="48" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="J12" s="31"/>
     </row>
@@ -7570,17 +7570,17 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>798</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>799</v>
       </c>
       <c r="F13" s="64"/>
       <c r="G13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="J13" s="31"/>
     </row>
@@ -7589,13 +7589,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>66</v>
@@ -7608,17 +7608,17 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
+        <v>775</v>
+      </c>
+      <c r="E15" s="31" t="s">
         <v>776</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>777</v>
       </c>
       <c r="F15" s="64"/>
       <c r="G15" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -7627,17 +7627,17 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>164</v>
       </c>
       <c r="F16" s="64"/>
       <c r="G16" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="J16" s="31"/>
     </row>
@@ -7646,17 +7646,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
+        <v>780</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>781</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>782</v>
       </c>
       <c r="F17" s="64"/>
       <c r="G17" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7665,14 +7665,14 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
+        <v>783</v>
+      </c>
+      <c r="E18" s="31" t="s">
         <v>784</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>785</v>
       </c>
       <c r="F18" s="64"/>
       <c r="G18" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I18" s="31" t="s">
         <v>648</v>
@@ -7684,17 +7684,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
+        <v>785</v>
+      </c>
+      <c r="E19" s="31" t="s">
         <v>786</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>787</v>
       </c>
       <c r="F19" s="64"/>
       <c r="G19" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="J19" s="31"/>
     </row>
@@ -7703,17 +7703,17 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
+        <v>722</v>
+      </c>
+      <c r="E20" s="31" t="s">
         <v>723</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>724</v>
       </c>
       <c r="F20" s="64"/>
       <c r="G20" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I20" s="48" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J20" s="31"/>
     </row>
@@ -7722,17 +7722,17 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
+        <v>724</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>725</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>726</v>
       </c>
       <c r="F21" s="64"/>
       <c r="G21" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I21" s="48" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J21" s="31"/>
     </row>
@@ -7741,17 +7741,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="E22" s="31" t="s">
         <v>789</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>790</v>
       </c>
       <c r="F22" s="64"/>
       <c r="G22" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -7760,13 +7760,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>231</v>
@@ -7818,7 +7818,7 @@
         <v>22</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>68</v>
@@ -7847,7 +7847,7 @@
         <v>1</v>
       </c>
       <c r="R26" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7855,10 +7855,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="30" t="s">
+        <v>668</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>669</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>670</v>
       </c>
       <c r="F27" s="64"/>
       <c r="G27" s="30" t="s">
@@ -7873,10 +7873,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E28" s="56" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F28" s="64"/>
       <c r="G28" s="56" t="s">
@@ -7901,8 +7901,8 @@
       <c r="O28" s="58">
         <v>0.01</v>
       </c>
-      <c r="R28" s="56" t="s">
-        <v>652</v>
+      <c r="R28" s="40" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7910,10 +7910,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F29" s="64"/>
       <c r="G29" s="30" t="s">
@@ -7928,10 +7928,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F30" s="65"/>
       <c r="G30" s="30" t="s">
@@ -8048,7 +8048,7 @@
         <v>21</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E36" s="52" t="s">
         <v>44</v>
@@ -8078,8 +8078,8 @@
         <v>1</v>
       </c>
       <c r="Q36" s="55"/>
-      <c r="R36" s="52" t="s">
-        <v>652</v>
+      <c r="R36" s="40" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -8314,7 +8314,7 @@
         <v>22</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E46" s="40" t="s">
         <v>286</v>
@@ -8324,7 +8324,7 @@
         <v>62</v>
       </c>
       <c r="H46" s="40" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I46" s="40">
         <v>0</v>
@@ -8347,7 +8347,7 @@
         <v>1</v>
       </c>
       <c r="R46" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8355,7 +8355,7 @@
         <v>21</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E47" s="30" t="s">
         <v>46</v>
@@ -8365,7 +8365,7 @@
         <v>62</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I47" s="30">
         <v>0</v>
@@ -8376,7 +8376,7 @@
         <v>21</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E48" s="30" t="s">
         <v>48</v>
@@ -8386,7 +8386,7 @@
         <v>62</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I48" s="30">
         <v>0</v>
@@ -8397,7 +8397,7 @@
         <v>21</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E49" s="30" t="s">
         <v>50</v>
@@ -8407,7 +8407,7 @@
         <v>63</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I49" s="30">
         <v>0</v>
@@ -8418,7 +8418,7 @@
         <v>21</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E50" s="30" t="s">
         <v>52</v>
@@ -8436,7 +8436,7 @@
         <v>21</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E51" s="30" t="s">
         <v>54</v>
@@ -8446,7 +8446,7 @@
         <v>63</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I51" s="30">
         <v>15</v>
@@ -8457,7 +8457,7 @@
         <v>21</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E52" s="30" t="s">
         <v>56</v>
@@ -8467,7 +8467,7 @@
         <v>62</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I52" s="30">
         <v>0</v>
@@ -8478,7 +8478,7 @@
         <v>21</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E53" s="30" t="s">
         <v>58</v>
@@ -8488,7 +8488,7 @@
         <v>63</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I53" s="30">
         <v>1</v>
@@ -8499,13 +8499,13 @@
         <v>1</v>
       </c>
       <c r="B54" s="46" t="s">
+        <v>746</v>
+      </c>
+      <c r="C54" s="46" t="s">
         <v>747</v>
       </c>
-      <c r="C54" s="46" t="s">
-        <v>748</v>
-      </c>
       <c r="D54" s="46" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E54" s="46" t="s">
         <v>66</v>
@@ -8537,17 +8537,17 @@
         <v>22</v>
       </c>
       <c r="D56" s="40" t="s">
+        <v>748</v>
+      </c>
+      <c r="E56" s="40" t="s">
         <v>749</v>
-      </c>
-      <c r="E56" s="40" t="s">
-        <v>750</v>
       </c>
       <c r="F56" s="50"/>
       <c r="G56" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H56" s="40" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I56" s="40">
         <v>0.8</v>
@@ -8570,7 +8570,7 @@
         <v>1</v>
       </c>
       <c r="R56" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8596,7 +8596,7 @@
         <v>21</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E58" s="30" t="s">
         <v>126</v>
@@ -8606,7 +8606,7 @@
         <v>62</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I58" s="30">
         <v>0</v>
@@ -8617,7 +8617,7 @@
         <v>21</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E59" s="30" t="s">
         <v>48</v>
@@ -8627,7 +8627,7 @@
         <v>62</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I59" s="30">
         <v>0</v>
@@ -8638,7 +8638,7 @@
         <v>21</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E60" s="30" t="s">
         <v>50</v>
@@ -8648,7 +8648,7 @@
         <v>63</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I60" s="30">
         <v>0</v>
@@ -8659,7 +8659,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E61" s="30" t="s">
         <v>52</v>
@@ -8677,7 +8677,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E62" s="30" t="s">
         <v>54</v>
@@ -8687,7 +8687,7 @@
         <v>63</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I62" s="30">
         <v>15</v>
@@ -8698,7 +8698,7 @@
         <v>21</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E63" s="30" t="s">
         <v>56</v>
@@ -8708,7 +8708,7 @@
         <v>62</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I63" s="30">
         <v>0</v>
@@ -8719,7 +8719,7 @@
         <v>21</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>58</v>
@@ -8729,7 +8729,7 @@
         <v>63</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I64" s="30">
         <v>1</v>
@@ -8740,13 +8740,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C65" s="46" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D65" s="46" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E65" s="46" t="s">
         <v>66</v>
@@ -8757,7 +8757,7 @@
         <v>21</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E66" s="30" t="s">
         <v>124</v>
@@ -8778,17 +8778,17 @@
         <v>22</v>
       </c>
       <c r="D67" s="40" t="s">
+        <v>755</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>756</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>757</v>
       </c>
       <c r="F67" s="50"/>
       <c r="G67" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H67" s="40" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I67" s="40">
         <v>4</v>
@@ -8811,7 +8811,7 @@
         <v>0.25</v>
       </c>
       <c r="R67" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8837,7 +8837,7 @@
         <v>21</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E69" s="30" t="s">
         <v>126</v>
@@ -8847,7 +8847,7 @@
         <v>62</v>
       </c>
       <c r="H69" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I69" s="30">
         <v>0</v>
@@ -8858,7 +8858,7 @@
         <v>21</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E70" s="30" t="s">
         <v>48</v>
@@ -8868,7 +8868,7 @@
         <v>62</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I70" s="30">
         <v>0</v>
@@ -8879,7 +8879,7 @@
         <v>21</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E71" s="30" t="s">
         <v>50</v>
@@ -8889,7 +8889,7 @@
         <v>63</v>
       </c>
       <c r="H71" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I71" s="30">
         <v>0</v>
@@ -8900,7 +8900,7 @@
         <v>21</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E72" s="30" t="s">
         <v>52</v>
@@ -8918,7 +8918,7 @@
         <v>21</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E73" s="30" t="s">
         <v>54</v>
@@ -8928,7 +8928,7 @@
         <v>63</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I73" s="30">
         <v>15</v>
@@ -8939,7 +8939,7 @@
         <v>21</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E74" s="30" t="s">
         <v>56</v>
@@ -8949,7 +8949,7 @@
         <v>62</v>
       </c>
       <c r="H74" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I74" s="30">
         <v>0</v>
@@ -8960,7 +8960,7 @@
         <v>21</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E75" s="30" t="s">
         <v>58</v>
@@ -8970,7 +8970,7 @@
         <v>63</v>
       </c>
       <c r="H75" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I75" s="30">
         <v>1</v>
@@ -9019,7 +9019,7 @@
         <v>22</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>243</v>
@@ -9029,7 +9029,7 @@
         <v>62</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I78" s="40">
         <v>0</v>
@@ -9052,7 +9052,7 @@
         <v>1</v>
       </c>
       <c r="R78" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="79" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9060,17 +9060,17 @@
         <v>22</v>
       </c>
       <c r="D79" s="40" t="s">
+        <v>758</v>
+      </c>
+      <c r="E79" s="40" t="s">
         <v>759</v>
-      </c>
-      <c r="E79" s="40" t="s">
-        <v>760</v>
       </c>
       <c r="F79" s="50"/>
       <c r="G79" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I79" s="40">
         <v>0</v>
@@ -9093,7 +9093,7 @@
         <v>1</v>
       </c>
       <c r="R79" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9119,7 +9119,7 @@
         <v>21</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E81" s="30" t="s">
         <v>126</v>
@@ -9129,7 +9129,7 @@
         <v>62</v>
       </c>
       <c r="H81" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I81" s="30">
         <v>0</v>
@@ -9140,7 +9140,7 @@
         <v>21</v>
       </c>
       <c r="D82" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E82" s="30" t="s">
         <v>48</v>
@@ -9150,7 +9150,7 @@
         <v>62</v>
       </c>
       <c r="H82" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I82" s="30">
         <v>0</v>
@@ -9161,7 +9161,7 @@
         <v>21</v>
       </c>
       <c r="D83" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E83" s="30" t="s">
         <v>50</v>
@@ -9171,7 +9171,7 @@
         <v>63</v>
       </c>
       <c r="H83" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I83" s="30">
         <v>0</v>
@@ -9182,7 +9182,7 @@
         <v>21</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E84" s="30" t="s">
         <v>52</v>
@@ -9200,7 +9200,7 @@
         <v>21</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E85" s="30" t="s">
         <v>54</v>
@@ -9210,7 +9210,7 @@
         <v>63</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I85" s="30">
         <v>15</v>
@@ -9221,7 +9221,7 @@
         <v>21</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E86" s="30" t="s">
         <v>56</v>
@@ -9231,7 +9231,7 @@
         <v>62</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I86" s="30">
         <v>0</v>
@@ -9242,7 +9242,7 @@
         <v>21</v>
       </c>
       <c r="D87" s="30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E87" s="30" t="s">
         <v>58</v>
@@ -9252,7 +9252,7 @@
         <v>63</v>
       </c>
       <c r="H87" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I87" s="30">
         <v>1</v>
@@ -9266,10 +9266,10 @@
         <v>185</v>
       </c>
       <c r="C88" s="46" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D88" s="46" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E88" s="46" t="s">
         <v>66</v>
@@ -9280,7 +9280,7 @@
         <v>22</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E89" s="40" t="s">
         <v>188</v>
@@ -9290,7 +9290,7 @@
         <v>62</v>
       </c>
       <c r="H89" s="40" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I89" s="40">
         <v>0</v>
@@ -9313,7 +9313,7 @@
         <v>1</v>
       </c>
       <c r="R89" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="90" spans="1:20" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9321,7 +9321,7 @@
         <v>22</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E90" s="40" t="s">
         <v>190</v>
@@ -9331,7 +9331,7 @@
         <v>62</v>
       </c>
       <c r="H90" s="40" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I90" s="40">
         <v>0</v>
@@ -9354,7 +9354,7 @@
         <v>1</v>
       </c>
       <c r="R90" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
@@ -9362,7 +9362,7 @@
         <v>21</v>
       </c>
       <c r="D91" s="31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E91" s="31" t="s">
         <v>192</v>
@@ -9379,19 +9379,20 @@
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
+      <c r="R91" s="40"/>
     </row>
     <row r="92" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="49" t="b">
         <v>1</v>
       </c>
       <c r="B92" s="49" t="s">
+        <v>732</v>
+      </c>
+      <c r="C92" s="49" t="s">
         <v>733</v>
       </c>
-      <c r="C92" s="49" t="s">
-        <v>734</v>
-      </c>
       <c r="D92" s="49" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E92" s="46" t="s">
         <v>66</v>
@@ -9417,10 +9418,10 @@
       </c>
       <c r="C93" s="50"/>
       <c r="D93" s="50" t="s">
+        <v>726</v>
+      </c>
+      <c r="E93" s="50" t="s">
         <v>727</v>
-      </c>
-      <c r="E93" s="50" t="s">
-        <v>728</v>
       </c>
       <c r="F93" s="50"/>
       <c r="G93" s="50" t="s">
@@ -9450,7 +9451,7 @@
       <c r="P93" s="40"/>
       <c r="Q93" s="40"/>
       <c r="R93" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="94" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9460,10 +9461,10 @@
       </c>
       <c r="C94" s="50"/>
       <c r="D94" s="50" t="s">
+        <v>728</v>
+      </c>
+      <c r="E94" s="50" t="s">
         <v>729</v>
-      </c>
-      <c r="E94" s="50" t="s">
-        <v>730</v>
       </c>
       <c r="F94" s="50"/>
       <c r="G94" s="50" t="s">
@@ -9492,7 +9493,7 @@
       <c r="P94" s="40"/>
       <c r="Q94" s="40"/>
       <c r="R94" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="95" spans="1:20" s="30" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9502,10 +9503,10 @@
       </c>
       <c r="C95" s="50"/>
       <c r="D95" s="50" t="s">
+        <v>730</v>
+      </c>
+      <c r="E95" s="50" t="s">
         <v>731</v>
-      </c>
-      <c r="E95" s="50" t="s">
-        <v>732</v>
       </c>
       <c r="F95" s="50"/>
       <c r="G95" s="50" t="s">
@@ -9534,7 +9535,7 @@
       <c r="P95" s="42"/>
       <c r="Q95" s="42"/>
       <c r="R95" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
       <c r="T95" s="31"/>
     </row>
@@ -9543,13 +9544,13 @@
         <v>1</v>
       </c>
       <c r="B96" s="49" t="s">
+        <v>734</v>
+      </c>
+      <c r="C96" s="49" t="s">
         <v>735</v>
       </c>
-      <c r="C96" s="49" t="s">
-        <v>736</v>
-      </c>
       <c r="D96" s="49" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E96" s="46" t="s">
         <v>66</v>
@@ -9575,10 +9576,10 @@
       </c>
       <c r="C97" s="50"/>
       <c r="D97" s="50" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E97" s="50" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F97" s="50"/>
       <c r="G97" s="50" t="s">
@@ -9608,7 +9609,7 @@
       <c r="P97" s="40"/>
       <c r="Q97" s="40"/>
       <c r="R97" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9618,10 +9619,10 @@
       </c>
       <c r="C98" s="50"/>
       <c r="D98" s="50" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E98" s="50" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F98" s="50"/>
       <c r="G98" s="50" t="s">
@@ -9650,7 +9651,7 @@
       <c r="P98" s="40"/>
       <c r="Q98" s="40"/>
       <c r="R98" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9660,10 +9661,10 @@
       </c>
       <c r="C99" s="50"/>
       <c r="D99" s="50" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E99" s="50" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F99" s="50"/>
       <c r="G99" s="50" t="s">
@@ -9692,7 +9693,7 @@
       <c r="P99" s="42"/>
       <c r="Q99" s="42"/>
       <c r="R99" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9700,13 +9701,13 @@
         <v>1</v>
       </c>
       <c r="B100" s="46" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C100" s="46" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D100" s="46" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E100" s="46" t="s">
         <v>66</v>
@@ -9717,17 +9718,17 @@
         <v>21</v>
       </c>
       <c r="D101" s="56" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E101" s="56" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F101" s="64"/>
       <c r="G101" s="56" t="s">
         <v>62</v>
       </c>
       <c r="H101" s="56" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I101" s="56">
         <v>1</v>
@@ -9749,8 +9750,8 @@
       <c r="O101" s="58">
         <v>0.1</v>
       </c>
-      <c r="R101" s="56" t="s">
-        <v>652</v>
+      <c r="R101" s="40" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9758,17 +9759,17 @@
         <v>22</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E102" s="40" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F102" s="50"/>
       <c r="G102" s="40" t="s">
         <v>62</v>
       </c>
       <c r="H102" s="40" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I102" s="40">
         <v>1450</v>
@@ -9791,7 +9792,7 @@
         <v>50</v>
       </c>
       <c r="R102" s="40" t="s">
-        <v>652</v>
+        <v>820</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -9799,13 +9800,13 @@
         <v>1</v>
       </c>
       <c r="B103" s="37" t="s">
+        <v>739</v>
+      </c>
+      <c r="C103" s="37" t="s">
         <v>740</v>
       </c>
-      <c r="C103" s="37" t="s">
-        <v>741</v>
-      </c>
       <c r="D103" s="37" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E103" s="37" t="s">
         <v>231</v>
@@ -10281,7 +10282,7 @@
         <v>457</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>630</v>
@@ -10319,7 +10320,7 @@
         <v>622</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>635</v>
@@ -10417,7 +10418,7 @@
         <v>639</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>634</v>
@@ -10449,7 +10450,7 @@
         <v>640</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>633</v>
@@ -10478,12 +10479,12 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>466</v>
@@ -10507,12 +10508,12 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>466</v>
@@ -10536,12 +10537,12 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>466</v>
@@ -10564,12 +10565,12 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E11" s="30" t="s">
         <v>466</v>
@@ -10592,12 +10593,12 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>466</v>
@@ -10620,12 +10621,12 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>466</v>
@@ -10648,12 +10649,12 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="30"/>
       <c r="D14" s="30" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>466</v>
@@ -10677,12 +10678,12 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>466</v>
@@ -10706,12 +10707,12 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>466</v>
@@ -10735,12 +10736,12 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>466</v>
@@ -10764,12 +10765,12 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>466</v>
@@ -10793,12 +10794,12 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>466</v>
@@ -10822,12 +10823,12 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>466</v>
@@ -10851,12 +10852,12 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E21" s="30" t="s">
         <v>466</v>
@@ -10880,15 +10881,15 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="30"/>
       <c r="D22" s="30" t="s">
+        <v>706</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>707</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>708</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>62</v>
@@ -10909,15 +10910,15 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>62</v>
@@ -10938,15 +10939,15 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>62</v>
@@ -10967,15 +10968,15 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B25" s="47"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30" t="s">
+        <v>713</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>714</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>715</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>62</v>
@@ -11001,7 +11002,7 @@
       <c r="B26" s="47"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>646</v>
@@ -11030,7 +11031,7 @@
       <c r="B27" s="47"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>648</v>
@@ -11054,15 +11055,15 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>62</v>
@@ -11082,15 +11083,15 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>62</v>
@@ -11110,15 +11111,15 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
       <c r="D30" s="30" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>62</v>
@@ -11138,15 +11139,15 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>62</v>
@@ -11166,15 +11167,15 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>62</v>
@@ -11194,15 +11195,15 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>62</v>
@@ -11222,12 +11223,12 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
       <c r="D34" s="30" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E34" s="30"/>
       <c r="F34" s="31" t="s">
@@ -11245,12 +11246,12 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="30" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E35" s="30"/>
       <c r="F35" s="31" t="s">
@@ -11268,12 +11269,12 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="30" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E36" s="30"/>
       <c r="F36" s="31" t="s">
@@ -11291,11 +11292,11 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B37" s="30"/>
       <c r="D37" s="30" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
update spreadsheets to nokogiri fixed AMIs rollback analysis gem to be compatible with AMIs (no skip or docker support)
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -2493,7 +2493,7 @@
     <t>uniform</t>
   </si>
   <si>
-    <t>1.17.0</t>
+    <t>1.21.14</t>
   </si>
 </sst>
 </file>
@@ -6790,7 +6790,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6908,7 +6908,7 @@
         <v>456</v>
       </c>
       <c r="B9" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="32"/>

</xml_diff>

<commit_message>
more tests for 2.0
</commit_message>
<xml_diff>
--- a/projects/SEB_LHS_2013.xlsx
+++ b/projects/SEB_LHS_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2439,45 +2439,6 @@
     <t>SEB4 baseboard LHS 2013 184</t>
   </si>
   <si>
-    <t>CalibrationReportsEnhanced</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_nmbe_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_nmbe_within_limit</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -2488,6 +2449,45 @@
   </si>
   <si>
     <t>1.21.14</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_consumption_modeled</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_consumption_modeled</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_rmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_rmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20</t>
   </si>
 </sst>
 </file>
@@ -6783,7 +6783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -6842,7 +6842,7 @@
         <v>465</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>609</v>
@@ -6853,7 +6853,7 @@
         <v>466</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>812</v>
+        <v>799</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>468</v>
@@ -7195,9 +7195,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7721,13 +7721,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>799</v>
+        <v>815</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>799</v>
+        <v>815</v>
       </c>
       <c r="E23" s="36" t="s">
         <v>231</v>
@@ -7808,7 +7808,7 @@
         <v>1</v>
       </c>
       <c r="R26" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -7863,7 +7863,7 @@
         <v>0.01</v>
       </c>
       <c r="R28" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -8040,7 +8040,7 @@
       </c>
       <c r="Q36" s="54"/>
       <c r="R36" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -8308,7 +8308,7 @@
         <v>1</v>
       </c>
       <c r="R46" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8531,7 +8531,7 @@
         <v>1</v>
       </c>
       <c r="R56" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -8772,7 +8772,7 @@
         <v>0.25</v>
       </c>
       <c r="R67" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9013,7 +9013,7 @@
         <v>1</v>
       </c>
       <c r="R78" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="79" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9054,7 +9054,7 @@
         <v>1</v>
       </c>
       <c r="R79" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9274,7 +9274,7 @@
         <v>1</v>
       </c>
       <c r="R89" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="90" spans="1:20" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9315,7 +9315,7 @@
         <v>1</v>
       </c>
       <c r="R90" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
@@ -9412,7 +9412,7 @@
       <c r="P93" s="39"/>
       <c r="Q93" s="39"/>
       <c r="R93" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="94" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9454,7 +9454,7 @@
       <c r="P94" s="39"/>
       <c r="Q94" s="39"/>
       <c r="R94" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="95" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9496,7 +9496,7 @@
       <c r="P95" s="41"/>
       <c r="Q95" s="41"/>
       <c r="R95" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="T95" s="30"/>
     </row>
@@ -9570,7 +9570,7 @@
       <c r="P97" s="39"/>
       <c r="Q97" s="39"/>
       <c r="R97" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9612,7 +9612,7 @@
       <c r="P98" s="39"/>
       <c r="Q98" s="39"/>
       <c r="R98" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9654,7 +9654,7 @@
       <c r="P99" s="41"/>
       <c r="Q99" s="41"/>
       <c r="R99" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9712,7 +9712,7 @@
         <v>0.1</v>
       </c>
       <c r="R101" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9753,7 +9753,7 @@
         <v>50</v>
       </c>
       <c r="R102" s="39" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -10953,7 +10953,7 @@
       <c r="B26" s="46"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>643</v>
@@ -10982,7 +10982,7 @@
       <c r="B27" s="46"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>645</v>
@@ -11011,7 +11011,7 @@
       <c r="B28" s="46"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>651</v>
@@ -11039,7 +11039,7 @@
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>651</v>
@@ -11067,7 +11067,7 @@
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>651</v>
@@ -11095,7 +11095,7 @@
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>651</v>
@@ -11123,7 +11123,7 @@
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>651</v>
@@ -11151,7 +11151,7 @@
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>651</v>
@@ -11179,7 +11179,7 @@
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="30" t="s">
@@ -11202,7 +11202,7 @@
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
       <c r="D35" s="29" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="30" t="s">
@@ -11225,7 +11225,7 @@
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
       <c r="D36" s="29" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="30" t="s">
@@ -11247,7 +11247,7 @@
       </c>
       <c r="B37" s="29"/>
       <c r="D37" s="29" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="F37" s="30" t="s">
         <v>62</v>

</xml_diff>